<commit_message>
Quick save at Mon Aug 29 18:09:30 UTC 2016
</commit_message>
<xml_diff>
--- a/tools/irradiation.xlsx
+++ b/tools/irradiation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27800" windowHeight="14380" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,12 @@
     <sheet name="DSP" sheetId="7" r:id="rId6"/>
     <sheet name="LOG" sheetId="4" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -218,7 +223,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +256,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -288,11 +309,85 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -340,9 +435,83 @@
     <xf numFmtId="11" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="78">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -359,7 +528,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -431,22 +600,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>6.3694267515923563E-11</c:v>
+                    <c:v>6.36942675159235E-11</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6257583550696438E-9</c:v>
+                    <c:v>1.62575835506964E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.2440983795165841E-8</c:v>
+                    <c:v>2.24409837951658E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.5350766839171053E-8</c:v>
+                    <c:v>1.53507668391711E-8</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.9229597646525798E-8</c:v>
+                    <c:v>1.92295976465258E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.0765537461360367E-8</c:v>
+                    <c:v>2.07655374613604E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -458,22 +627,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>6.3694267515923563E-11</c:v>
+                    <c:v>6.36942675159235E-11</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6257583550696438E-9</c:v>
+                    <c:v>1.62575835506964E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.2440983795165841E-8</c:v>
+                    <c:v>2.24409837951658E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.5350766839171053E-8</c:v>
+                    <c:v>1.53507668391711E-8</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.9229597646525798E-8</c:v>
+                    <c:v>1.92295976465258E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.0765537461360367E-8</c:v>
+                    <c:v>2.07655374613604E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -484,7 +653,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -502,13 +671,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>40.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -520,22 +689,22 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.3694267515923563E-11</c:v>
+                  <c:v>6.36942675159235E-11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.4747406749023928E-9</c:v>
+                  <c:v>9.4747406749024E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7177345855534705E-7</c:v>
+                  <c:v>1.71773458555347E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1325966850828727E-7</c:v>
+                  <c:v>2.13259668508287E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5690258150125591E-7</c:v>
+                  <c:v>2.56902581501256E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0780339936267451E-7</c:v>
+                  <c:v>3.07803399362674E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -573,22 +742,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.3490721165139769E-11</c:v>
+                    <c:v>2.34907211651398E-11</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.5558446618079027E-9</c:v>
+                    <c:v>5.5558446618079E-9</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.5559178183620553E-9</c:v>
+                    <c:v>4.55591781836205E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.4878104158114532E-9</c:v>
+                    <c:v>5.48781041581145E-9</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>6.6351466991058516E-9</c:v>
+                    <c:v>6.63514669910585E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -600,22 +769,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.3490721165139769E-11</c:v>
+                    <c:v>2.34907211651398E-11</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.5558446618079027E-9</c:v>
+                    <c:v>5.5558446618079E-9</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.5559178183620553E-9</c:v>
+                    <c:v>4.55591781836205E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.4878104158114532E-9</c:v>
+                    <c:v>5.48781041581145E-9</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>6.6351466991058516E-9</c:v>
+                    <c:v>6.63514669910585E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -626,7 +795,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -644,13 +813,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>40.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -662,22 +831,22 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3490721165139769E-11</c:v>
+                  <c:v>2.34907211651398E-11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.1899682620874422E-9</c:v>
+                  <c:v>7.18996826208744E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.878453038674033E-8</c:v>
+                  <c:v>1.87845303867403E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1310120831168684E-8</c:v>
+                  <c:v>2.13101208311687E-8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1866601323241053E-8</c:v>
+                  <c:v>3.1866601323241E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -692,11 +861,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115867648"/>
-        <c:axId val="115868224"/>
+        <c:axId val="-2146174984"/>
+        <c:axId val="-2146178120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115867648"/>
+        <c:axId val="-2146174984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -706,12 +875,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115868224"/>
+        <c:crossAx val="-2146178120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115868224"/>
+        <c:axId val="-2146178120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,7 +891,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115867648"/>
+        <c:crossAx val="-2146174984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -747,7 +916,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -814,25 +983,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>1.6901312987870707E-8</c:v>
+                    <c:v>1.69013129878707E-8</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.3777436815212472E-8</c:v>
+                    <c:v>2.37774368152125E-8</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.8803006218930324E-8</c:v>
+                    <c:v>1.88030062189303E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.3503169784073593E-8</c:v>
+                    <c:v>2.35031697840736E-8</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.2328463449322545E-8</c:v>
+                    <c:v>2.23284634493225E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.4204377713617443E-8</c:v>
+                    <c:v>1.42043777136174E-8</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.657893611789101E-8</c:v>
+                    <c:v>1.6578936117891E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -844,25 +1013,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>1.6901312987870707E-8</c:v>
+                    <c:v>1.69013129878707E-8</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.3777436815212472E-8</c:v>
+                    <c:v>2.37774368152125E-8</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.8803006218930324E-8</c:v>
+                    <c:v>1.88030062189303E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.3503169784073593E-8</c:v>
+                    <c:v>2.35031697840736E-8</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.2328463449322545E-8</c:v>
+                    <c:v>2.23284634493225E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.4204377713617443E-8</c:v>
+                    <c:v>1.42043777136174E-8</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.657893611789101E-8</c:v>
+                    <c:v>1.6578936117891E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -873,7 +1042,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -912,25 +1081,25 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.4080664294187427E-7</c:v>
+                  <c:v>2.40806642941874E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4480369515011545E-7</c:v>
+                  <c:v>2.44803695150115E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7506426735218507E-7</c:v>
+                  <c:v>2.75064267352185E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9166666666666664E-7</c:v>
+                  <c:v>2.91666666666667E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7071823204419894E-7</c:v>
+                  <c:v>2.70718232044199E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1588785046728975E-7</c:v>
+                  <c:v>2.1588785046729E-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3967889908256879E-7</c:v>
+                  <c:v>2.39678899082569E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -968,25 +1137,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>6.2769900618376997E-9</c:v>
+                    <c:v>6.2769900618377E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.3031816632064184E-9</c:v>
+                    <c:v>7.30318166320642E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.9781276943540061E-9</c:v>
+                    <c:v>4.97812769435401E-9</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.5607985135184749E-9</c:v>
+                    <c:v>6.56079851351847E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.8237157645826517E-9</c:v>
+                    <c:v>5.82371576458265E-9</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>4.1795663130837192E-9</c:v>
+                    <c:v>4.17956631308372E-9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>4.5871559633027526E-9</c:v>
+                    <c:v>4.58715596330275E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -998,25 +1167,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>6.2769900618376997E-9</c:v>
+                    <c:v>6.2769900618377E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.3031816632064184E-9</c:v>
+                    <c:v>7.30318166320642E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.9781276943540061E-9</c:v>
+                    <c:v>4.97812769435401E-9</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.5607985135184749E-9</c:v>
+                    <c:v>6.56079851351847E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.8237157645826517E-9</c:v>
+                    <c:v>5.82371576458265E-9</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>4.1795663130837192E-9</c:v>
+                    <c:v>4.17956631308372E-9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>4.5871559633027526E-9</c:v>
+                    <c:v>4.58715596330275E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1027,7 +1196,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1066,25 +1235,25 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.3214709371293001E-8</c:v>
+                  <c:v>3.3214709371293E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3094688221709007E-8</c:v>
+                  <c:v>2.3094688221709E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9280205655526991E-8</c:v>
+                  <c:v>1.9280205655527E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2727272727272725E-8</c:v>
+                  <c:v>2.27272727272727E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.841620626151013E-8</c:v>
+                  <c:v>1.84162062615101E-8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8691588785046729E-8</c:v>
+                  <c:v>1.86915887850467E-8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.834862385321101E-8</c:v>
+                  <c:v>1.8348623853211E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1099,11 +1268,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115870528"/>
-        <c:axId val="115871104"/>
+        <c:axId val="-2144714296"/>
+        <c:axId val="-2144711096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115870528"/>
+        <c:axId val="-2144714296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1113,12 +1282,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115871104"/>
+        <c:crossAx val="-2144711096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115871104"/>
+        <c:axId val="-2144711096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,7 +1298,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115870528"/>
+        <c:crossAx val="-2144714296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1154,7 +1323,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1186,6 +1355,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1225,22 +1395,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.2488554743461749E-9</c:v>
+                    <c:v>1.24885547434617E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.0708351019586504E-8</c:v>
+                    <c:v>2.07083510195865E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.4408881163729623E-9</c:v>
+                    <c:v>9.44088811637296E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2314530656039954E-8</c:v>
+                    <c:v>1.231453065604E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.2244644926995123E-8</c:v>
+                    <c:v>1.22446449269951E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1252,22 +1422,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.2488554743461749E-9</c:v>
+                    <c:v>1.24885547434617E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.0708351019586504E-8</c:v>
+                    <c:v>2.07083510195865E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.4408881163729623E-9</c:v>
+                    <c:v>9.44088811637296E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2314530656039954E-8</c:v>
+                    <c:v>1.231453065604E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.2244644926995123E-8</c:v>
+                    <c:v>1.22446449269951E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1278,7 +1448,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1296,13 +1466,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>40.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1314,22 +1484,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1465588286388024E-8</c:v>
+                  <c:v>1.1465588286388E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.060393649675122E-7</c:v>
+                  <c:v>1.06039364967512E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.066298342541436E-8</c:v>
+                  <c:v>8.06629834254143E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0151070608044769E-7</c:v>
+                  <c:v>1.01510706080448E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.5676789436704994E-8</c:v>
+                  <c:v>9.5676789436705E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1367,22 +1537,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9138682956562178E-9</c:v>
+                    <c:v>1.91386829565622E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.3104946627845505E-10</c:v>
+                    <c:v>3.31049466278455E-10</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.5530200966281132E-9</c:v>
+                    <c:v>2.55302009662811E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1394,22 +1564,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9138682956562178E-9</c:v>
+                    <c:v>1.91386829565622E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.3104946627845505E-10</c:v>
+                    <c:v>3.31049466278455E-10</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.5530200966281132E-9</c:v>
+                    <c:v>2.55302009662811E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1420,7 +1590,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1438,13 +1608,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>40.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1456,22 +1626,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.314917127071823E-9</c:v>
+                  <c:v>3.31491712707182E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.7339449541284397E-10</c:v>
+                  <c:v>5.73394495412844E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7084188624970326E-8</c:v>
+                  <c:v>1.70841886249703E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1486,11 +1656,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115873408"/>
-        <c:axId val="115873984"/>
+        <c:axId val="-2146296712"/>
+        <c:axId val="-2146299848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115873408"/>
+        <c:axId val="-2146296712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1500,12 +1670,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115873984"/>
+        <c:crossAx val="-2146299848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115873984"/>
+        <c:axId val="-2146299848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1516,13 +1686,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115873408"/>
+        <c:crossAx val="-2146296712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1540,7 +1711,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1593,6 +1764,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1632,25 +1804,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>9.8200060126057377E-9</c:v>
+                    <c:v>9.82000601260573E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6330410650959527E-8</c:v>
+                    <c:v>1.63304106509595E-8</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.2328615741163802E-8</c:v>
+                    <c:v>1.23286157411638E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.4961396693620555E-8</c:v>
+                    <c:v>1.49613966936206E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>8.0395563243389032E-9</c:v>
+                    <c:v>8.0395563243389E-9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>9.5259447969243979E-9</c:v>
+                    <c:v>9.5259447969244E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1662,25 +1834,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>9.8200060126057377E-9</c:v>
+                    <c:v>9.82000601260573E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6330410650959527E-8</c:v>
+                    <c:v>1.63304106509595E-8</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.2328615741163802E-8</c:v>
+                    <c:v>1.23286157411638E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.4961396693620555E-8</c:v>
+                    <c:v>1.49613966936206E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>8.0395563243389032E-9</c:v>
+                    <c:v>8.0395563243389E-9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>9.5259447969243979E-9</c:v>
+                    <c:v>9.5259447969244E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1691,7 +1863,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1730,25 +1902,25 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>8.4474885844748857E-8</c:v>
+                  <c:v>8.44748858447488E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1547344110854504E-7</c:v>
+                  <c:v>1.15473441108545E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1825192802056555E-7</c:v>
+                  <c:v>1.18251928020566E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2154696132596685E-7</c:v>
+                  <c:v>1.21546961325967E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9158878504672909E-8</c:v>
+                  <c:v>6.91588785046729E-8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.9128440366972472E-8</c:v>
+                  <c:v>7.91284403669725E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1786,25 +1958,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>4.4212138655335807E-9</c:v>
+                    <c:v>4.42121386553358E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.9862967976707304E-9</c:v>
+                    <c:v>1.98629679767073E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1816,25 +1988,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>4.4212138655335807E-9</c:v>
+                    <c:v>4.42121386553358E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.9862967976707304E-9</c:v>
+                    <c:v>1.98629679767073E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1845,7 +2017,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1884,25 +2056,25 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.7123287671232876E-8</c:v>
+                  <c:v>1.71232876712329E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.440366972477064E-9</c:v>
+                  <c:v>3.44036697247706E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1917,11 +2089,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118456896"/>
-        <c:axId val="118457472"/>
+        <c:axId val="-2146339080"/>
+        <c:axId val="-2146342280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118456896"/>
+        <c:axId val="-2146339080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1931,12 +2103,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118457472"/>
+        <c:crossAx val="-2146342280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118457472"/>
+        <c:axId val="-2146342280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1947,13 +2119,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118456896"/>
+        <c:crossAx val="-2146339080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2387,26 +2560,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" style="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1">
       <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
@@ -2440,7 +2613,7 @@
       <c r="L1"/>
       <c r="M1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2474,7 +2647,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2510,7 +2683,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2546,7 +2719,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2582,7 +2755,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2618,7 +2791,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2654,7 +2827,7 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="19">
         <v>7</v>
       </c>
@@ -2690,7 +2863,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="19">
         <v>8</v>
       </c>
@@ -2726,7 +2899,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -2762,7 +2935,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="19">
         <v>10</v>
       </c>
@@ -2798,7 +2971,7 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="19">
         <v>11</v>
       </c>
@@ -2834,7 +3007,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="19">
         <v>12</v>
       </c>
@@ -2870,7 +3043,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="19">
         <v>13</v>
       </c>
@@ -2906,7 +3079,7 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="19">
         <v>14</v>
       </c>
@@ -2942,7 +3115,7 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="19">
         <v>15</v>
       </c>
@@ -2978,7 +3151,7 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="19">
         <v>16</v>
       </c>
@@ -3014,7 +3187,7 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="19">
         <v>17</v>
       </c>
@@ -3050,7 +3223,7 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -3086,7 +3259,7 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="19">
         <v>19</v>
       </c>
@@ -3122,7 +3295,7 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="19">
         <v>20</v>
       </c>
@@ -3158,7 +3331,7 @@
       </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="19">
         <v>21</v>
       </c>
@@ -3194,7 +3367,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -3230,7 +3403,7 @@
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="19">
         <v>23</v>
       </c>
@@ -3266,7 +3439,7 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="19">
         <v>24</v>
       </c>
@@ -3302,7 +3475,7 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="19">
         <v>25</v>
       </c>
@@ -3338,7 +3511,7 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="19">
         <v>26</v>
       </c>
@@ -3374,7 +3547,7 @@
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="19">
         <v>27</v>
       </c>
@@ -3410,7 +3583,7 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="19">
         <v>28</v>
       </c>
@@ -3446,7 +3619,7 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="19">
         <v>29</v>
       </c>
@@ -3482,7 +3655,7 @@
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="19">
         <v>30</v>
       </c>
@@ -3518,7 +3691,7 @@
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="19">
         <v>31</v>
       </c>
@@ -3554,7 +3727,7 @@
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="19">
         <v>32</v>
       </c>
@@ -3590,7 +3763,7 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="19">
         <v>33</v>
       </c>
@@ -3626,7 +3799,7 @@
       </c>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="19">
         <v>34</v>
       </c>
@@ -3662,7 +3835,7 @@
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="19">
         <v>35</v>
       </c>
@@ -3698,7 +3871,7 @@
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="19">
         <v>36</v>
       </c>
@@ -3734,7 +3907,7 @@
       </c>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="19">
         <v>37</v>
       </c>
@@ -3770,7 +3943,7 @@
       </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="19">
         <v>38</v>
       </c>
@@ -3806,7 +3979,7 @@
       </c>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" s="19">
         <v>39</v>
       </c>
@@ -3842,7 +4015,7 @@
       </c>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="19">
         <v>40</v>
       </c>
@@ -3878,7 +4051,7 @@
       </c>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="19">
         <v>41</v>
       </c>
@@ -3914,21 +4087,21 @@
       </c>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="C43"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="C44"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="B45" s="4"/>
       <c r="C45"/>
       <c r="E45" s="5"/>
@@ -3936,43 +4109,48 @@
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="C46"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="C47"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="C48"/>
     </row>
-    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" ht="14.25" customHeight="1">
       <c r="C49"/>
     </row>
-    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" ht="14.25" customHeight="1">
       <c r="C50"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3">
       <c r="C51"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3">
       <c r="C52"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3">
       <c r="C53"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3">
       <c r="C54"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3">
       <c r="C55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3984,29 +4162,29 @@
       <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -4062,7 +4240,7 @@
       <c r="AA1"/>
       <c r="AB1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -4107,7 +4285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -4156,7 +4334,7 @@
       </c>
       <c r="P3" s="8"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -4205,7 +4383,7 @@
       </c>
       <c r="P4" s="9"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -4254,7 +4432,7 @@
       </c>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -4301,7 +4479,7 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -4346,7 +4524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -4391,7 +4569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -4436,7 +4614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -4481,7 +4659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -4526,7 +4704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" s="11" customFormat="1">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -4571,7 +4749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -4616,7 +4794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -4661,7 +4839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -4715,7 +4893,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -4775,7 +4953,7 @@
         <v>2694339186.25</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -4834,7 +5012,7 @@
         <v>93.38886304694509</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -4879,7 +5057,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -4924,7 +5102,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -4969,7 +5147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -5014,7 +5192,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -5059,7 +5237,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -5104,7 +5282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -5149,7 +5327,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -5194,7 +5372,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -5239,7 +5417,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -5284,7 +5462,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -5329,7 +5507,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -5374,7 +5552,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -5419,7 +5597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -5464,7 +5642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -5512,7 +5690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -5557,7 +5735,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -5602,7 +5780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -5613,7 +5791,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -5658,7 +5836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -5669,7 +5847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -5714,7 +5892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -5725,7 +5903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -5770,7 +5948,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -5781,7 +5959,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -5826,19 +6004,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14">
       <c r="A47"/>
       <c r="C47"/>
       <c r="D47"/>
@@ -5852,7 +6030,7 @@
       <c r="L47"/>
       <c r="M47"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14">
       <c r="A48"/>
       <c r="C48"/>
       <c r="D48"/>
@@ -5866,7 +6044,7 @@
       <c r="L48"/>
       <c r="M48"/>
     </row>
-    <row r="49" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="14.25" customHeight="1">
       <c r="A49"/>
       <c r="C49"/>
       <c r="D49"/>
@@ -5880,7 +6058,7 @@
       <c r="L49"/>
       <c r="M49"/>
     </row>
-    <row r="50" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="14.25" customHeight="1">
       <c r="A50"/>
       <c r="C50"/>
       <c r="D50"/>
@@ -5894,7 +6072,7 @@
       <c r="L50"/>
       <c r="M50"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51"/>
       <c r="C51"/>
       <c r="D51"/>
@@ -5908,7 +6086,7 @@
       <c r="L51"/>
       <c r="M51"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13">
       <c r="A52"/>
       <c r="C52"/>
       <c r="D52"/>
@@ -5922,7 +6100,7 @@
       <c r="L52"/>
       <c r="M52"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="A53"/>
       <c r="C53"/>
       <c r="D53"/>
@@ -5936,7 +6114,7 @@
       <c r="L53"/>
       <c r="M53"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="A54"/>
       <c r="C54"/>
       <c r="D54"/>
@@ -5950,7 +6128,7 @@
       <c r="L54"/>
       <c r="M54"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13">
       <c r="A55"/>
       <c r="C55"/>
       <c r="D55"/>
@@ -5966,6 +6144,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5973,28 +6156,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N23" sqref="N23:N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -6035,7 +6218,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -6087,7 +6270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -6140,7 +6323,7 @@
         <v>2.3490721165139769E-11</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -6193,7 +6376,7 @@
         <v>5.5558446618079027E-9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -6246,7 +6429,7 @@
         <v>4.5559178183620553E-9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -6299,7 +6482,7 @@
         <v>5.4878104158114532E-9</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -6355,7 +6538,7 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -6392,7 +6575,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -6430,7 +6613,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -6465,7 +6648,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -6500,7 +6683,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -6533,7 +6716,7 @@
         <v>3.1948881789137384E-10</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -6568,7 +6751,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -6603,7 +6786,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -6638,7 +6821,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -6673,7 +6856,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -6708,7 +6891,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -6743,7 +6926,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -6778,7 +6961,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -6813,7 +6996,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -6848,7 +7031,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -6897,7 +7080,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -6951,7 +7134,7 @@
         <v>6.2769900618376997E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -7005,7 +7188,7 @@
         <v>7.3031816632064184E-9</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -7059,7 +7242,7 @@
         <v>4.9781276943540061E-9</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -7113,7 +7296,7 @@
         <v>6.5607985135184749E-9</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -7167,7 +7350,7 @@
         <v>5.8237157645826517E-9</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -7221,7 +7404,7 @@
         <v>4.1795663130837192E-9</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -7275,7 +7458,7 @@
         <v>4.5871559633027526E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -7314,7 +7497,7 @@
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -7353,7 +7536,7 @@
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -7392,7 +7575,7 @@
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -7427,7 +7610,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -7462,7 +7645,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -7497,7 +7680,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -7532,7 +7715,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -7567,7 +7750,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -7602,7 +7785,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -7637,7 +7820,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -7672,7 +7855,7 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -7707,7 +7890,7 @@
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -7744,7 +7927,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7756,20 +7945,20 @@
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -7801,7 +7990,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -7842,7 +8031,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -7883,7 +8072,7 @@
         <v>5.8681146350119296E-10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -7924,7 +8113,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -7965,7 +8154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -8006,7 +8195,7 @@
         <v>6.6453948290016432E-9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -8047,7 +8236,7 @@
         <v>4.3520033314593927E-9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -8088,7 +8277,7 @@
         <v>5.9857447747829428E-9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -8129,7 +8318,7 @@
         <v>2.5901762193934272E-9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -8170,7 +8359,7 @@
         <v>4.6681470996122009E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -8211,7 +8400,7 @@
         <v>6.2648681882412326E-9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -8252,7 +8441,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -8293,7 +8482,7 @@
         <v>4.5391131461693942E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -8334,7 +8523,7 @@
         <v>1.7803769385032856E-7</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -8375,7 +8564,7 @@
         <v>5.4110859468596274E-8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -8416,7 +8605,7 @@
         <v>2.1049365817823592E-9</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -8457,7 +8646,7 @@
         <v>1.4488502372054678E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -8498,7 +8687,7 @@
         <v>1.5160239930406474E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -8539,7 +8728,7 @@
         <v>1.7768347980735624E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -8580,7 +8769,7 @@
         <v>6.249507209650355E-8</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -8621,7 +8810,7 @@
         <v>2.1730325425903627E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -8662,7 +8851,7 @@
         <v>1.6738026719384817E-7</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -8703,7 +8892,7 @@
         <v>2.4192229502593938E-7</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -8744,7 +8933,7 @@
         <v>1.0829418898901413E-7</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -8785,7 +8974,7 @@
         <v>1.6284462085529774E-7</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -8826,7 +9015,7 @@
         <v>1.984838479972653E-7</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -8867,7 +9056,7 @@
         <v>2.0273050531062635E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -8908,7 +9097,7 @@
         <v>1.1501684632164908E-7</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -8949,7 +9138,7 @@
         <v>4.4995057454511165E-8</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -8990,7 +9179,7 @@
         <v>2.4023841356392838E-7</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -9031,7 +9220,7 @@
         <v>1.4169938870962971E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -9072,7 +9261,7 @@
         <v>2.7163596069493577E-7</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -9113,7 +9302,7 @@
         <v>3.0560203715755513E-7</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -9154,7 +9343,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -9195,7 +9384,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -9236,7 +9425,7 @@
         <v>6.8184834679892083E-8</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -9277,7 +9466,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -9318,7 +9507,7 @@
         <v>1.4456958633214434E-7</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -9359,7 +9548,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -9400,7 +9589,7 @@
         <v>1.5607330098029108E-7</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -9441,7 +9630,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -9482,47 +9671,52 @@
         <v>1.958220015922994E-7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9530,27 +9724,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23:N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -9591,7 +9785,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -9643,7 +9837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -9695,7 +9889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -9747,7 +9941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -9800,7 +9994,7 @@
       </c>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -9852,7 +10046,7 @@
         <v>3.3104946627845505E-10</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -9904,7 +10098,7 @@
         <v>2.5530200966281132E-9</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -9937,7 +10131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -9972,7 +10166,7 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -10008,7 +10202,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -10041,7 +10235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -10074,7 +10268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -10107,7 +10301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -10140,7 +10334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="21">
         <v>14</v>
       </c>
@@ -10173,7 +10367,7 @@
         <v>2.042409173267478E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -10206,7 +10400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -10239,7 +10433,7 @@
         <v>1.9138682956562178E-9</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" s="21">
         <v>17</v>
       </c>
@@ -10272,7 +10466,7 @@
         <v>2.1937416380672515E-8</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -10305,7 +10499,7 @@
         <v>4.4212138655335807E-9</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -10338,7 +10532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="21">
         <v>20</v>
       </c>
@@ -10371,7 +10565,7 @@
         <v>1.3346158677408842E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -10419,7 +10613,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -10472,7 +10666,7 @@
         <v>4.4212138655335807E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="21">
         <v>23</v>
       </c>
@@ -10525,7 +10719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -10578,7 +10772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="21">
         <v>25</v>
       </c>
@@ -10631,7 +10825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -10684,7 +10878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -10737,7 +10931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="21">
         <v>28</v>
       </c>
@@ -10790,7 +10984,7 @@
         <v>1.9862967976707304E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -10823,7 +11017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -10856,7 +11050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -10890,7 +11084,7 @@
       </c>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -10923,7 +11117,7 @@
         <v>8.3466982961670055E-9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -10956,7 +11150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -10989,7 +11183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="21">
         <v>35</v>
       </c>
@@ -11022,7 +11216,7 @@
         <v>7.9466275527930666E-7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -11055,7 +11249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -11088,7 +11282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -11121,7 +11315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -11154,7 +11348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -11187,7 +11381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -11222,8 +11416,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -11235,19 +11434,19 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -11265,7 +11464,7 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -11282,7 +11481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -11299,7 +11498,7 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -11316,7 +11515,7 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -11333,7 +11532,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -11350,7 +11549,7 @@
         <v>4.2300000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -11367,7 +11566,7 @@
         <v>7.54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -11384,7 +11583,7 @@
         <v>13.19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -11401,7 +11600,7 @@
         <v>14.69</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -11418,7 +11617,7 @@
         <v>17.989999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -11435,7 +11634,7 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="11" customFormat="1">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -11452,7 +11651,7 @@
         <v>22.74</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -11469,7 +11668,7 @@
         <v>24.03</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -11486,7 +11685,7 @@
         <v>24.05</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -11503,7 +11702,7 @@
         <v>24.35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -11520,7 +11719,7 @@
         <v>24.73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -11537,7 +11736,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -11554,7 +11753,7 @@
         <v>25.04</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -11571,7 +11770,7 @@
         <v>25.15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -11588,7 +11787,7 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -11605,7 +11804,7 @@
         <v>25.29</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -11622,7 +11821,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -11639,7 +11838,7 @@
         <v>25.47</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -11656,7 +11855,7 @@
         <v>25.55</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -11673,7 +11872,7 @@
         <v>25.64</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -11690,7 +11889,7 @@
         <v>25.73</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -11707,7 +11906,7 @@
         <v>25.81</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -11724,7 +11923,7 @@
         <v>25.95</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -11741,7 +11940,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -11758,7 +11957,7 @@
         <v>26.22</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -11775,7 +11974,7 @@
         <v>26.55</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -11792,7 +11991,7 @@
         <v>26.67</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -11809,7 +12008,7 @@
         <v>26.83</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -11826,7 +12025,7 @@
         <v>33.43</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -11843,7 +12042,7 @@
         <v>43.43</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -11860,7 +12059,7 @@
         <v>43.51</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -11877,7 +12076,7 @@
         <v>53.52</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -11894,7 +12093,7 @@
         <v>53.61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -11911,7 +12110,7 @@
         <v>63.61</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -11928,7 +12127,7 @@
         <v>63.78</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -11945,7 +12144,7 @@
         <v>83.82</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -11962,48 +12161,53 @@
         <v>83.96</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -12015,21 +12219,21 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1">
         <v>23</v>
       </c>
@@ -12061,7 +12265,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>24</v>
       </c>
@@ -12093,7 +12297,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>25</v>
       </c>
@@ -12125,7 +12329,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>26</v>
       </c>
@@ -12157,7 +12361,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>27</v>
       </c>
@@ -12189,7 +12393,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>28</v>
       </c>
@@ -12221,7 +12425,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>29</v>
       </c>
@@ -12253,7 +12457,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>30</v>
       </c>
@@ -12285,7 +12489,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>31</v>
       </c>
@@ -12317,7 +12521,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>32</v>
       </c>
@@ -12349,7 +12553,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>33</v>
       </c>
@@ -12381,7 +12585,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>34</v>
       </c>
@@ -12413,7 +12617,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>35</v>
       </c>
@@ -12445,7 +12649,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>36</v>
       </c>
@@ -12477,7 +12681,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>37</v>
       </c>
@@ -12509,7 +12713,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>38</v>
       </c>
@@ -12541,7 +12745,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>39</v>
       </c>
@@ -12573,7 +12777,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>40</v>
       </c>
@@ -12605,7 +12809,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>41</v>
       </c>
@@ -12640,7 +12844,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>59</v>
       </c>
@@ -12672,7 +12876,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>60</v>
       </c>
@@ -12704,7 +12908,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>61</v>
       </c>
@@ -12736,7 +12940,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>62</v>
       </c>
@@ -12768,7 +12972,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>63</v>
       </c>
@@ -12800,7 +13004,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>64</v>
       </c>
@@ -12832,7 +13036,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>65</v>
       </c>
@@ -12864,7 +13068,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>66</v>
       </c>
@@ -12896,7 +13100,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>67</v>
       </c>
@@ -12928,7 +13132,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>68</v>
       </c>
@@ -12960,7 +13164,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>69</v>
       </c>
@@ -12992,7 +13196,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>70</v>
       </c>
@@ -13024,7 +13228,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>71</v>
       </c>
@@ -13056,7 +13260,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>72</v>
       </c>
@@ -13088,7 +13292,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>73</v>
       </c>
@@ -13120,7 +13324,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>74</v>
       </c>
@@ -13152,7 +13356,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>75</v>
       </c>
@@ -13184,7 +13388,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>76</v>
       </c>
@@ -13216,7 +13420,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>77</v>
       </c>
@@ -13248,7 +13452,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>78</v>
       </c>
@@ -13280,7 +13484,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>79</v>
       </c>
@@ -13312,7 +13516,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>80</v>
       </c>
@@ -13344,7 +13548,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>81</v>
       </c>
@@ -13376,7 +13580,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>82</v>
       </c>
@@ -13408,7 +13612,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>83</v>
       </c>
@@ -13442,5 +13646,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Quick save at mer. 31/08/2016_17:04:16,94
</commit_message>
<xml_diff>
--- a/tools/irradiation.xlsx
+++ b/tools/irradiation.xlsx
@@ -1065,11 +1065,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53545216"/>
-        <c:axId val="53545792"/>
+        <c:axId val="116589120"/>
+        <c:axId val="116589696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53545216"/>
+        <c:axId val="116589120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1079,12 +1079,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53545792"/>
+        <c:crossAx val="116589696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53545792"/>
+        <c:axId val="116589696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1095,7 +1095,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53545216"/>
+        <c:crossAx val="116589120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1472,11 +1472,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53548096"/>
-        <c:axId val="53548672"/>
+        <c:axId val="116592000"/>
+        <c:axId val="116592576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53548096"/>
+        <c:axId val="116592000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1486,12 +1486,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53548672"/>
+        <c:crossAx val="116592576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53548672"/>
+        <c:axId val="116592576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1502,7 +1502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53548096"/>
+        <c:crossAx val="116592000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2004,11 +2004,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45850624"/>
-        <c:axId val="45851200"/>
+        <c:axId val="116594880"/>
+        <c:axId val="116595456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45850624"/>
+        <c:axId val="116594880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2018,12 +2018,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45851200"/>
+        <c:crossAx val="116595456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45851200"/>
+        <c:axId val="116595456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2034,7 +2034,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45850624"/>
+        <c:crossAx val="116594880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2437,11 +2437,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45853504"/>
-        <c:axId val="45854080"/>
+        <c:axId val="117687424"/>
+        <c:axId val="117688000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45853504"/>
+        <c:axId val="117687424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,12 +2451,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45854080"/>
+        <c:crossAx val="117688000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45854080"/>
+        <c:axId val="117688000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2467,7 +2467,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45853504"/>
+        <c:crossAx val="117687424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8048,8 +8048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9097,7 +9097,7 @@
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -9148,7 +9148,7 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -9199,7 +9199,7 @@
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -9250,7 +9250,7 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -9301,7 +9301,7 @@
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -9352,7 +9352,7 @@
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -9417,7 +9417,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -9487,7 +9487,7 @@
         <v>6.2769900618376997E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -9557,7 +9557,7 @@
         <v>7.3031816632064184E-9</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -9626,8 +9626,12 @@
         <f t="shared" si="18"/>
         <v>4.9781276943540061E-9</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T25" s="5">
+        <f>O7*1000*60*60*24</f>
+        <v>26.594213704935076</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -9697,7 +9701,7 @@
         <v>6.5607985135184749E-9</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -9767,7 +9771,7 @@
         <v>5.8237157645826517E-9</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -9837,7 +9841,7 @@
         <v>4.1795663130837192E-9</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -9907,7 +9911,7 @@
         <v>4.5871559633027526E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -9962,7 +9966,7 @@
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -10017,7 +10021,7 @@
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -10598,8 +10602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Quick save at jeu. 01/09/2016_11:55:06,72
</commit_message>
<xml_diff>
--- a/tools/irradiation.xlsx
+++ b/tools/irradiation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14385" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14385" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="84">
   <si>
     <t>Time</t>
   </si>
@@ -257,6 +257,27 @@
   </si>
   <si>
     <t>Error Single 2</t>
+  </si>
+  <si>
+    <t>1E6 - 5E6</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>5E6-1E7</t>
+  </si>
+  <si>
+    <t>5E5-1E6</t>
+  </si>
+  <si>
+    <t>&gt; 1E7</t>
+  </si>
+  <si>
+    <t>&lt; 5E5</t>
   </si>
 </sst>
 </file>
@@ -1065,11 +1086,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116589120"/>
-        <c:axId val="116589696"/>
+        <c:axId val="117113408"/>
+        <c:axId val="117113984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116589120"/>
+        <c:axId val="117113408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1079,12 +1100,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116589696"/>
+        <c:crossAx val="117113984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116589696"/>
+        <c:axId val="117113984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1095,7 +1116,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116589120"/>
+        <c:crossAx val="117113408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1472,11 +1493,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116592000"/>
-        <c:axId val="116592576"/>
+        <c:axId val="117116288"/>
+        <c:axId val="117116864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116592000"/>
+        <c:axId val="117116288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1486,12 +1507,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116592576"/>
+        <c:crossAx val="117116864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116592576"/>
+        <c:axId val="117116864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1502,7 +1523,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116592000"/>
+        <c:crossAx val="117116288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2004,11 +2025,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116594880"/>
-        <c:axId val="116595456"/>
+        <c:axId val="117119168"/>
+        <c:axId val="117119744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116594880"/>
+        <c:axId val="117119168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2018,12 +2039,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116595456"/>
+        <c:crossAx val="117119744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116595456"/>
+        <c:axId val="117119744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2034,7 +2055,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116594880"/>
+        <c:crossAx val="117119168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2437,11 +2458,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="117687424"/>
-        <c:axId val="117688000"/>
+        <c:axId val="118211712"/>
+        <c:axId val="118212288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="117687424"/>
+        <c:axId val="118211712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,12 +2472,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117688000"/>
+        <c:crossAx val="118212288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="117688000"/>
+        <c:axId val="118212288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2467,7 +2488,222 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117687424"/>
+        <c:crossAx val="118211712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CLB!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>L1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:strRef>
+              <c:f>CLB!$K$3:$K$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>&lt; 5E5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5E5-1E6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E6 - 5E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5E6-1E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>&gt; 1E7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CLB!$L$3:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>81.388340359171622</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.102856559998202</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.775772621870921</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.995380204515513</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CLB!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>L2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:strRef>
+              <c:f>CLB!$K$3:$K$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>&lt; 5E5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5E5-1E6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E6 - 5E6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5E6-1E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>&gt; 1E7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CLB!$M$3:$M$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>18.611659640828378</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.897143440001798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.224227378129093</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.004619795484487</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="120295936"/>
+        <c:axId val="75852032"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="120295936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75852032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="75852032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120295936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2611,6 +2847,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1142999</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2909,7 +3180,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4507,7 +4778,7 @@
   <dimension ref="A1:AB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6505,7 +6776,7 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8048,7 +8319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
@@ -13072,10 +13343,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13091,7 +13362,7 @@
     <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -13123,7 +13394,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -13163,8 +13434,14 @@
         <f>E2*G2/100/Parameters!$C2/Parameters!$G2</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -13204,8 +13481,19 @@
         <f>E3*G3/100/Parameters!$C3/Parameters!$G3</f>
         <v>5.8681146350119296E-10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3">
+        <f>AVERAGE(F24,F5)</f>
+        <v>81.388340359171622</v>
+      </c>
+      <c r="M3">
+        <f>AVERAGE(G24,G5)</f>
+        <v>18.611659640828378</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -13245,8 +13533,19 @@
         <f>E4*G4/100/Parameters!$C4/Parameters!$G4</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L4">
+        <f>AVERAGE(F5,F22,F24,F33)</f>
+        <v>51.102856559998202</v>
+      </c>
+      <c r="M4">
+        <f>AVERAGE(G5,G22,G24,G33)</f>
+        <v>48.897143440001798</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -13286,8 +13585,19 @@
         <f>E5*G5/100/Parameters!$C5/Parameters!$G5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5">
+        <f>AVERAGE(F6,F7,F8,F15,F16,F20,F21,F23,F25,F27,F26,F32,F36,F40)</f>
+        <v>43.775772621870921</v>
+      </c>
+      <c r="M5">
+        <f>AVERAGE(G6,G7,G8,G15,G16,G20,G21,G23,G25,G27,G26,G32,G36,G40)</f>
+        <v>56.224227378129093</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -13327,8 +13637,19 @@
         <f>E6*G6/100/Parameters!$C6/Parameters!$G6</f>
         <v>6.6453948290016432E-9</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6">
+        <f>AVERAGE(F10,F11,F13,F14,F17,F18,F19,F28,F30,F31,F38)</f>
+        <v>27.995380204515513</v>
+      </c>
+      <c r="M6">
+        <f>AVERAGE(G10,G11,G13,G14,G17,G18,G19,G28,G30,G31,G38)</f>
+        <v>72.004619795484487</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -13368,8 +13689,17 @@
         <f>E7*G7/100/Parameters!$C7/Parameters!$G7</f>
         <v>4.3520033314593927E-9</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -13410,19 +13740,19 @@
         <v>5.9857447747829428E-9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9">
         <f>Parameters!D9</f>
         <v>20.5</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="5">
         <f>Parameters!G9</f>
         <v>4601167.3151750974</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="5">
         <f>Parameters!J9</f>
         <v>14.69</v>
       </c>
@@ -13451,7 +13781,7 @@
         <v>2.5901762193934272E-9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -13492,7 +13822,7 @@
         <v>4.6681470996122009E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -13533,19 +13863,19 @@
         <v>6.2648681882412326E-9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12">
         <f>Parameters!D12</f>
         <v>20.5</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="5">
         <f>Parameters!G12</f>
         <v>5064724.919093851</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="5">
         <f>Parameters!J12</f>
         <v>22.74</v>
       </c>
@@ -13561,20 +13891,20 @@
         <f>Data!M12/(Data!$L12+Data!$M12)*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="14">
         <f>E12/Parameters!$C12/Parameters!$G12</f>
         <v>0</v>
       </c>
-      <c r="I12" s="1" t="e">
+      <c r="I12" s="14" t="e">
         <f>E12*F12/100/Parameters!$C12/Parameters!$G12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J12" s="1" t="e">
+      <c r="J12" s="14" t="e">
         <f>E12*G12/100/Parameters!$C12/Parameters!$G12</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -13615,7 +13945,7 @@
         <v>4.5391131461693942E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -13656,7 +13986,7 @@
         <v>1.7803769385032856E-7</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -13697,7 +14027,7 @@
         <v>5.4110859468596274E-8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -14845,6 +15175,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Quick save at ven. 02/09/2016_11:55:12,63
</commit_message>
<xml_diff>
--- a/tools/irradiation.xlsx
+++ b/tools/irradiation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27800" windowHeight="14380" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="DSP" sheetId="7" r:id="rId7"/>
     <sheet name="LOG" sheetId="4" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -654,7 +654,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -720,22 +720,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>6.36942675159235E-11</c:v>
+                    <c:v>6.3694267515923563E-11</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.62575835506964E-9</c:v>
+                    <c:v>1.6257583550696438E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.24409837951658E-8</c:v>
+                    <c:v>2.2440983795165841E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.53507668391711E-8</c:v>
+                    <c:v>1.5350766839171053E-8</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.92295976465258E-8</c:v>
+                    <c:v>1.9229597646525798E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.07655374613604E-8</c:v>
+                    <c:v>2.0765537461360367E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -747,22 +747,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>6.36942675159235E-11</c:v>
+                    <c:v>6.3694267515923563E-11</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.62575835506964E-9</c:v>
+                    <c:v>1.6257583550696438E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.24409837951658E-8</c:v>
+                    <c:v>2.2440983795165841E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.53507668391711E-8</c:v>
+                    <c:v>1.5350766839171053E-8</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.92295976465258E-8</c:v>
+                    <c:v>1.9229597646525798E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.07655374613604E-8</c:v>
+                    <c:v>2.0765537461360367E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -773,7 +773,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1.0"/>
+            <c:val val="1"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -791,13 +791,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.8</c:v>
+                  <c:v>40.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -809,22 +809,22 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.36942675159235E-11</c:v>
+                  <c:v>6.3694267515923563E-11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.4747406749024E-9</c:v>
+                  <c:v>9.4747406749023928E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.71773458555347E-7</c:v>
+                  <c:v>1.7177345855534705E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.13259668508287E-7</c:v>
+                  <c:v>2.1325966850828727E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.56902581501256E-7</c:v>
+                  <c:v>2.5690258150125591E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.07803399362674E-7</c:v>
+                  <c:v>3.0780339936267451E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -862,22 +862,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.34907211651398E-11</c:v>
+                    <c:v>2.3490721165139769E-11</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.5558446618079E-9</c:v>
+                    <c:v>5.5558446618079027E-9</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.55591781836205E-9</c:v>
+                    <c:v>4.5559178183620553E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.48781041581145E-9</c:v>
+                    <c:v>5.4878104158114532E-9</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>6.63514669910585E-9</c:v>
+                    <c:v>6.6351466991058516E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -889,22 +889,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.34907211651398E-11</c:v>
+                    <c:v>2.3490721165139769E-11</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.5558446618079E-9</c:v>
+                    <c:v>5.5558446618079027E-9</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.55591781836205E-9</c:v>
+                    <c:v>4.5559178183620553E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.48781041581145E-9</c:v>
+                    <c:v>5.4878104158114532E-9</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>6.63514669910585E-9</c:v>
+                    <c:v>6.6351466991058516E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -915,7 +915,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1.0"/>
+            <c:val val="1"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -933,13 +933,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.8</c:v>
+                  <c:v>40.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -951,22 +951,22 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.34907211651398E-11</c:v>
+                  <c:v>2.3490721165139769E-11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.18996826208744E-9</c:v>
+                  <c:v>7.1899682620874422E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.87845303867403E-8</c:v>
+                  <c:v>1.878453038674033E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.13101208311687E-8</c:v>
+                  <c:v>2.1310120831168684E-8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1866601323241E-8</c:v>
+                  <c:v>3.1866601323241053E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1008,13 +1008,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.8</c:v>
+                  <c:v>40.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1026,19 +1026,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>1.27388535031847E-10</c:v>
+                  <c:v>1.2738853503184713E-10</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>1.54320987654321E-10</c:v>
+                  <c:v>1.5432098765432101E-10</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>2.76243093922652E-8</c:v>
+                  <c:v>2.7624309392265192E-8</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>1.53913538309976E-7</c:v>
+                  <c:v>1.5391353830997568E-7</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>2.57240567723302E-7</c:v>
+                  <c:v>2.5724056772330217E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,13 +1080,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.8</c:v>
+                  <c:v>40.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1098,19 +1098,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>4.87232301069873E-9</c:v>
+                  <c:v>4.8723230106987318E-9</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>2.38146603252035E-8</c:v>
+                  <c:v>2.3814660325203556E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1125,11 +1125,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2088641288"/>
-        <c:axId val="2088644504"/>
+        <c:axId val="114493120"/>
+        <c:axId val="114493696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2088641288"/>
+        <c:axId val="114493120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1139,12 +1139,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088644504"/>
+        <c:crossAx val="114493696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2088644504"/>
+        <c:axId val="114493696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,7 +1155,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088641288"/>
+        <c:crossAx val="114493120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1179,7 +1179,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1245,25 +1245,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>1.69013129878707E-8</c:v>
+                    <c:v>1.6901312987870707E-8</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.37774368152125E-8</c:v>
+                    <c:v>2.3777436815212472E-8</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.88030062189303E-8</c:v>
+                    <c:v>1.8803006218930324E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.35031697840736E-8</c:v>
+                    <c:v>2.3503169784073593E-8</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.23284634493225E-8</c:v>
+                    <c:v>2.2328463449322545E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.42043777136174E-8</c:v>
+                    <c:v>1.4204377713617443E-8</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.6578936117891E-8</c:v>
+                    <c:v>1.657893611789101E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1275,25 +1275,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>1.69013129878707E-8</c:v>
+                    <c:v>1.6901312987870707E-8</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.37774368152125E-8</c:v>
+                    <c:v>2.3777436815212472E-8</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.88030062189303E-8</c:v>
+                    <c:v>1.8803006218930324E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.35031697840736E-8</c:v>
+                    <c:v>2.3503169784073593E-8</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.23284634493225E-8</c:v>
+                    <c:v>2.2328463449322545E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.42043777136174E-8</c:v>
+                    <c:v>1.4204377713617443E-8</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.6578936117891E-8</c:v>
+                    <c:v>1.657893611789101E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1304,7 +1304,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1.0"/>
+            <c:val val="1"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1343,25 +1343,25 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.40806642941874E-7</c:v>
+                  <c:v>2.4080664294187427E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.44803695150115E-7</c:v>
+                  <c:v>2.4480369515011545E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.75064267352185E-7</c:v>
+                  <c:v>2.7506426735218507E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.91666666666667E-7</c:v>
+                  <c:v>2.9166666666666664E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.70718232044199E-7</c:v>
+                  <c:v>2.7071823204419894E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1588785046729E-7</c:v>
+                  <c:v>2.1588785046728975E-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.39678899082569E-7</c:v>
+                  <c:v>2.3967889908256879E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1399,25 +1399,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>6.2769900618377E-9</c:v>
+                    <c:v>6.2769900618376997E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.30318166320642E-9</c:v>
+                    <c:v>7.3031816632064184E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.97812769435401E-9</c:v>
+                    <c:v>4.9781276943540061E-9</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.56079851351847E-9</c:v>
+                    <c:v>6.5607985135184749E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.82371576458265E-9</c:v>
+                    <c:v>5.8237157645826517E-9</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>4.17956631308372E-9</c:v>
+                    <c:v>4.1795663130837192E-9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>4.58715596330275E-9</c:v>
+                    <c:v>4.5871559633027526E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1429,25 +1429,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>6.2769900618377E-9</c:v>
+                    <c:v>6.2769900618376997E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.30318166320642E-9</c:v>
+                    <c:v>7.3031816632064184E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.97812769435401E-9</c:v>
+                    <c:v>4.9781276943540061E-9</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.56079851351847E-9</c:v>
+                    <c:v>6.5607985135184749E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.82371576458265E-9</c:v>
+                    <c:v>5.8237157645826517E-9</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>4.17956631308372E-9</c:v>
+                    <c:v>4.1795663130837192E-9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>4.58715596330275E-9</c:v>
+                    <c:v>4.5871559633027526E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1458,7 +1458,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1.0"/>
+            <c:val val="1"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1497,25 +1497,25 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.3214709371293E-8</c:v>
+                  <c:v>3.3214709371293001E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3094688221709E-8</c:v>
+                  <c:v>2.3094688221709007E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9280205655527E-8</c:v>
+                  <c:v>1.9280205655526991E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.27272727272727E-8</c:v>
+                  <c:v>2.2727272727272725E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.84162062615101E-8</c:v>
+                  <c:v>1.841620626151013E-8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.86915887850467E-8</c:v>
+                  <c:v>1.8691588785046729E-8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8348623853211E-8</c:v>
+                  <c:v>1.834862385321101E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1530,11 +1530,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115644792"/>
-        <c:axId val="2115647992"/>
+        <c:axId val="114496000"/>
+        <c:axId val="114496576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115644792"/>
+        <c:axId val="114496000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1544,12 +1544,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115647992"/>
+        <c:crossAx val="114496576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2115647992"/>
+        <c:axId val="114496576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,7 +1560,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115644792"/>
+        <c:crossAx val="114496000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1584,7 +1584,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1655,22 +1655,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.24885547434617E-9</c:v>
+                    <c:v>1.2488554743461749E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.07083510195865E-8</c:v>
+                    <c:v>2.0708351019586504E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.44088811637296E-9</c:v>
+                    <c:v>9.4408881163729623E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.231453065604E-8</c:v>
+                    <c:v>1.2314530656039954E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.22446449269951E-8</c:v>
+                    <c:v>1.2244644926995123E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1682,22 +1682,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.24885547434617E-9</c:v>
+                    <c:v>1.2488554743461749E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.07083510195865E-8</c:v>
+                    <c:v>2.0708351019586504E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.44088811637296E-9</c:v>
+                    <c:v>9.4408881163729623E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.231453065604E-8</c:v>
+                    <c:v>1.2314530656039954E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.22446449269951E-8</c:v>
+                    <c:v>1.2244644926995123E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1708,7 +1708,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1.0"/>
+            <c:val val="1"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1726,13 +1726,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.8</c:v>
+                  <c:v>40.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1744,22 +1744,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1465588286388E-8</c:v>
+                  <c:v>1.1465588286388024E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.06039364967512E-7</c:v>
+                  <c:v>1.060393649675122E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.06629834254143E-8</c:v>
+                  <c:v>8.066298342541436E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.01510706080448E-7</c:v>
+                  <c:v>1.0151070608044769E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.5676789436705E-8</c:v>
+                  <c:v>9.5676789436704994E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1797,22 +1797,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.91386829565622E-9</c:v>
+                    <c:v>1.9138682956562178E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.31049466278455E-10</c:v>
+                    <c:v>3.3104946627845505E-10</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.55302009662811E-9</c:v>
+                    <c:v>2.5530200966281132E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1824,22 +1824,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.91386829565622E-9</c:v>
+                    <c:v>1.9138682956562178E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.31049466278455E-10</c:v>
+                    <c:v>3.3104946627845505E-10</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.55302009662811E-9</c:v>
+                    <c:v>2.5530200966281132E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1850,7 +1850,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1.0"/>
+            <c:val val="1"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1868,13 +1868,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.8</c:v>
+                  <c:v>40.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1886,22 +1886,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.31491712707182E-9</c:v>
+                  <c:v>3.314917127071823E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.73394495412844E-10</c:v>
+                  <c:v>5.7339449541284397E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.70841886249703E-8</c:v>
+                  <c:v>1.7084188624970326E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1943,13 +1943,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.8</c:v>
+                  <c:v>40.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1961,19 +1961,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.36942675159235E-11</c:v>
+                  <c:v>6.3694267515923563E-11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.98895027624309E-8</c:v>
+                  <c:v>1.9889502762430937E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.96428451088465E-8</c:v>
+                  <c:v>7.9642845108846474E-8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.26854604428382E-8</c:v>
+                  <c:v>9.2685460442838195E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2015,13 +2015,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.8</c:v>
+                  <c:v>40.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2033,19 +2033,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.04032946037509E-9</c:v>
+                  <c:v>1.0403294603750854E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2060,11 +2060,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2088714408"/>
-        <c:axId val="2088717560"/>
+        <c:axId val="114498880"/>
+        <c:axId val="114515968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2088714408"/>
+        <c:axId val="114498880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2074,12 +2074,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088717560"/>
+        <c:crossAx val="114515968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2088717560"/>
+        <c:axId val="114515968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2090,7 +2090,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088714408"/>
+        <c:crossAx val="114498880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2114,7 +2114,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2206,25 +2206,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>9.82000601260573E-9</c:v>
+                    <c:v>9.8200060126057377E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.63304106509595E-8</c:v>
+                    <c:v>1.6330410650959527E-8</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.23286157411638E-8</c:v>
+                    <c:v>1.2328615741163802E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.49613966936206E-8</c:v>
+                    <c:v>1.4961396693620555E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>8.0395563243389E-9</c:v>
+                    <c:v>8.0395563243389032E-9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>9.5259447969244E-9</c:v>
+                    <c:v>9.5259447969243979E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2236,25 +2236,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>9.82000601260573E-9</c:v>
+                    <c:v>9.8200060126057377E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.63304106509595E-8</c:v>
+                    <c:v>1.6330410650959527E-8</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.23286157411638E-8</c:v>
+                    <c:v>1.2328615741163802E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.49613966936206E-8</c:v>
+                    <c:v>1.4961396693620555E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>8.0395563243389E-9</c:v>
+                    <c:v>8.0395563243389032E-9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>9.5259447969244E-9</c:v>
+                    <c:v>9.5259447969243979E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2265,7 +2265,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1.0"/>
+            <c:val val="1"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -2304,25 +2304,25 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>8.44748858447488E-8</c:v>
+                  <c:v>8.4474885844748857E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.15473441108545E-7</c:v>
+                  <c:v>1.1547344110854504E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.18251928020566E-7</c:v>
+                  <c:v>1.1825192802056555E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.21546961325967E-7</c:v>
+                  <c:v>1.2154696132596685E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.91588785046729E-8</c:v>
+                  <c:v>6.9158878504672909E-8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.91284403669725E-8</c:v>
+                  <c:v>7.9128440366972472E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2360,25 +2360,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>4.42121386553358E-9</c:v>
+                    <c:v>4.4212138655335807E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.98629679767073E-9</c:v>
+                    <c:v>1.9862967976707304E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2390,25 +2390,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>4.42121386553358E-9</c:v>
+                    <c:v>4.4212138655335807E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.0</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.98629679767073E-9</c:v>
+                    <c:v>1.9862967976707304E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2419,7 +2419,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1.0"/>
+            <c:val val="1"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -2458,25 +2458,25 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.71232876712329E-8</c:v>
+                  <c:v>1.7123287671232876E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.44036697247706E-9</c:v>
+                  <c:v>3.440366972477064E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2491,11 +2491,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087834760"/>
-        <c:axId val="2087831560"/>
+        <c:axId val="114518272"/>
+        <c:axId val="114518848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2087834760"/>
+        <c:axId val="114518272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2505,12 +2505,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087831560"/>
+        <c:crossAx val="114518848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087831560"/>
+        <c:axId val="114518848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2521,7 +2521,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087834760"/>
+        <c:crossAx val="114518272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2545,7 +2545,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2611,19 +2611,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>81.38834035917162</c:v>
+                  <c:v>81.388340359171622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.1028565599982</c:v>
+                  <c:v>51.102856559998202</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.77577262187092</c:v>
+                  <c:v>43.775772621870921</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.99538020451551</c:v>
+                  <c:v>27.995380204515513</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2679,19 +2679,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18.61165964082838</c:v>
+                  <c:v>18.611659640828378</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.8971434400018</c:v>
+                  <c:v>48.897143440001798</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56.2242273781291</c:v>
+                  <c:v>56.224227378129093</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.00461979548448</c:v>
+                  <c:v>72.004619795484487</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2706,11 +2706,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087776600"/>
-        <c:axId val="2087773608"/>
+        <c:axId val="114521152"/>
+        <c:axId val="114521728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2087776600"/>
+        <c:axId val="114521152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2719,12 +2719,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087773608"/>
+        <c:crossAx val="114521728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087773608"/>
+        <c:axId val="114521728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2735,7 +2735,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087776600"/>
+        <c:crossAx val="114521152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3215,22 +3215,22 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.83203125" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
@@ -3264,7 +3264,7 @@
       <c r="L1"/>
       <c r="M1"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -3298,7 +3298,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -3334,7 +3334,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -3442,7 +3442,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>7</v>
       </c>
@@ -3514,7 +3514,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>8</v>
       </c>
@@ -3550,7 +3550,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -3586,7 +3586,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>10</v>
       </c>
@@ -3622,7 +3622,7 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>11</v>
       </c>
@@ -3658,7 +3658,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>12</v>
       </c>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>13</v>
       </c>
@@ -3730,7 +3730,7 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>14</v>
       </c>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>15</v>
       </c>
@@ -3802,7 +3802,7 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>16</v>
       </c>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>17</v>
       </c>
@@ -3874,7 +3874,7 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -3910,7 +3910,7 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>19</v>
       </c>
@@ -3946,7 +3946,7 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>20</v>
       </c>
@@ -3982,7 +3982,7 @@
       </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>21</v>
       </c>
@@ -4018,7 +4018,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -4054,7 +4054,7 @@
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>23</v>
       </c>
@@ -4090,7 +4090,7 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>24</v>
       </c>
@@ -4126,7 +4126,7 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>25</v>
       </c>
@@ -4162,7 +4162,7 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>26</v>
       </c>
@@ -4198,7 +4198,7 @@
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>27</v>
       </c>
@@ -4234,7 +4234,7 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
         <v>28</v>
       </c>
@@ -4270,7 +4270,7 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>29</v>
       </c>
@@ -4306,7 +4306,7 @@
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>30</v>
       </c>
@@ -4342,7 +4342,7 @@
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
         <v>31</v>
       </c>
@@ -4378,7 +4378,7 @@
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
         <v>32</v>
       </c>
@@ -4414,7 +4414,7 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
         <v>33</v>
       </c>
@@ -4450,7 +4450,7 @@
       </c>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
         <v>34</v>
       </c>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
         <v>35</v>
       </c>
@@ -4522,7 +4522,7 @@
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
         <v>36</v>
       </c>
@@ -4558,7 +4558,7 @@
       </c>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
         <v>37</v>
       </c>
@@ -4594,7 +4594,7 @@
       </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="19">
         <v>38</v>
       </c>
@@ -4630,7 +4630,7 @@
       </c>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
         <v>39</v>
       </c>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
         <v>40</v>
       </c>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="19">
         <v>41</v>
       </c>
@@ -4738,21 +4738,21 @@
       </c>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C43"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C44"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="C45"/>
       <c r="E45" s="5"/>
@@ -4760,38 +4760,38 @@
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C46"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C47"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C48"/>
     </row>
-    <row r="49" spans="3:3" ht="14.25" customHeight="1">
+    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49"/>
     </row>
-    <row r="50" spans="3:3" ht="14.25" customHeight="1">
+    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50"/>
     </row>
-    <row r="51" spans="3:3">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51"/>
     </row>
-    <row r="52" spans="3:3">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52"/>
     </row>
-    <row r="53" spans="3:3">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53"/>
     </row>
-    <row r="54" spans="3:3">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54"/>
     </row>
-    <row r="55" spans="3:3">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55"/>
     </row>
   </sheetData>
@@ -4809,33 +4809,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="3" customFormat="1">
+    <row r="1" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -4891,7 +4891,7 @@
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -4985,7 +4985,7 @@
       </c>
       <c r="P3" s="8"/>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -5034,7 +5034,7 @@
       </c>
       <c r="P4" s="9"/>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -5083,7 +5083,7 @@
       </c>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -5130,7 +5130,7 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="11" customFormat="1">
+    <row r="12" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>2694339186.25</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>93.38886304694509</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -5752,8 +5752,16 @@
       <c r="N19">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:19">
+      <c r="S19">
+        <f>S17/100*0.000000308</f>
+        <v>2.8763769818459089E-7</v>
+      </c>
+      <c r="T19">
+        <f>S19*1000*60*60*24</f>
+        <v>24.851897123148653</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -5797,8 +5805,16 @@
       <c r="N20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:19">
+      <c r="S20">
+        <f>Q17/100*0.000000308</f>
+        <v>2.0362301815409118E-8</v>
+      </c>
+      <c r="T20">
+        <f>S20*1000*60*60*24</f>
+        <v>1.7593028768513479</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -5843,7 +5859,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -5888,7 +5904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -5933,7 +5949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -5978,7 +5994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -6023,7 +6039,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -6068,7 +6084,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -6113,7 +6129,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -6158,7 +6174,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -6203,7 +6219,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -6248,7 +6264,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -6293,7 +6309,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -6341,7 +6357,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -6386,7 +6402,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -6431,7 +6447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -6442,7 +6458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -6487,7 +6503,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -6498,7 +6514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -6543,7 +6559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -6554,7 +6570,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -6599,7 +6615,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -6610,7 +6626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -6655,19 +6671,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="C47"/>
       <c r="D47"/>
@@ -6681,7 +6697,7 @@
       <c r="L47"/>
       <c r="M47"/>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="C48"/>
       <c r="D48"/>
@@ -6695,7 +6711,7 @@
       <c r="L48"/>
       <c r="M48"/>
     </row>
-    <row r="49" spans="1:13" ht="14.25" customHeight="1">
+    <row r="49" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="C49"/>
       <c r="D49"/>
@@ -6709,7 +6725,7 @@
       <c r="L49"/>
       <c r="M49"/>
     </row>
-    <row r="50" spans="1:13" ht="14.25" customHeight="1">
+    <row r="50" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50"/>
       <c r="C50"/>
       <c r="D50"/>
@@ -6723,7 +6739,7 @@
       <c r="L50"/>
       <c r="M50"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="C51"/>
       <c r="D51"/>
@@ -6737,7 +6753,7 @@
       <c r="L51"/>
       <c r="M51"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="C52"/>
       <c r="D52"/>
@@ -6751,7 +6767,7 @@
       <c r="L52"/>
       <c r="M52"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="C53"/>
       <c r="D53"/>
@@ -6765,7 +6781,7 @@
       <c r="L53"/>
       <c r="M53"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="C54"/>
       <c r="D54"/>
@@ -6779,7 +6795,7 @@
       <c r="L54"/>
       <c r="M54"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55"/>
       <c r="C55"/>
       <c r="D55"/>
@@ -6811,26 +6827,26 @@
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
     <col min="8" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="13.5" customWidth="1"/>
-    <col min="11" max="11" width="12.5" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" customWidth="1"/>
-    <col min="13" max="13" width="12.5" customWidth="1"/>
-    <col min="14" max="14" width="15.5" customWidth="1"/>
-    <col min="15" max="15" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1">
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -6875,7 +6891,7 @@
       </c>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -6895,7 +6911,7 @@
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -6915,7 +6931,7 @@
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -6935,7 +6951,7 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -6955,7 +6971,7 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -6975,7 +6991,7 @@
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -6995,7 +7011,7 @@
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -7015,7 +7031,7 @@
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -7035,7 +7051,7 @@
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -7055,7 +7071,7 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -7076,7 +7092,7 @@
       <c r="N11" s="11"/>
       <c r="O11" s="24"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -7097,7 +7113,7 @@
       <c r="N12" s="11"/>
       <c r="O12" s="24"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -7141,7 +7157,7 @@
       </c>
       <c r="O13" s="24"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -7185,7 +7201,7 @@
       </c>
       <c r="O14" s="24"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -7229,7 +7245,7 @@
       </c>
       <c r="O15" s="24"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -7271,7 +7287,7 @@
       </c>
       <c r="O16" s="24"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -7317,7 +7333,7 @@
       </c>
       <c r="O17" s="24"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -7363,7 +7379,7 @@
       </c>
       <c r="O18" s="24"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -7409,7 +7425,7 @@
       </c>
       <c r="O19" s="24"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -7455,7 +7471,7 @@
       </c>
       <c r="O20" s="24"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -7501,7 +7517,7 @@
       </c>
       <c r="O21" s="24"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -7547,7 +7563,7 @@
       </c>
       <c r="O22" s="24"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -7593,7 +7609,7 @@
       </c>
       <c r="O23" s="24"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -7639,7 +7655,7 @@
       </c>
       <c r="O24" s="24"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -7685,7 +7701,7 @@
       </c>
       <c r="O25" s="24"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -7731,7 +7747,7 @@
       </c>
       <c r="O26" s="24"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -7777,7 +7793,7 @@
       </c>
       <c r="O27" s="24"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -7823,7 +7839,7 @@
       </c>
       <c r="O28" s="24"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -7869,7 +7885,7 @@
       </c>
       <c r="O29" s="24"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -7915,7 +7931,7 @@
       </c>
       <c r="O30" s="24"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -7961,7 +7977,7 @@
       </c>
       <c r="O31" s="24"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -8007,7 +8023,7 @@
       </c>
       <c r="O32" s="24"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -8053,7 +8069,7 @@
       </c>
       <c r="O33" s="24"/>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -8097,7 +8113,7 @@
       <c r="N34" s="24"/>
       <c r="O34" s="24"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -8121,7 +8137,7 @@
       <c r="N35" s="24"/>
       <c r="O35" s="24"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -8167,7 +8183,7 @@
       </c>
       <c r="O36" s="24"/>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -8191,7 +8207,7 @@
       <c r="N37" s="24"/>
       <c r="O37" s="24"/>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -8236,7 +8252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -8259,7 +8275,7 @@
       <c r="M39" s="24"/>
       <c r="N39" s="24"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -8302,7 +8318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -8325,7 +8341,7 @@
       <c r="M41" s="24"/>
       <c r="N41" s="24"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -8355,32 +8371,32 @@
       <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -8445,7 +8461,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -8529,7 +8545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -8598,7 +8614,7 @@
         <v>2.3490721165139769E-11</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -8683,7 +8699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -8768,7 +8784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -8853,7 +8869,7 @@
         <v>2.6386406738987981E-9</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -8938,7 +8954,7 @@
         <v>5.6749155431643936E-9</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -8991,7 +9007,7 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -9045,7 +9061,7 @@
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -9096,7 +9112,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -9147,7 +9163,7 @@
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -9196,7 +9212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -9247,7 +9263,7 @@
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -9298,7 +9314,7 @@
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -9349,7 +9365,7 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -9400,7 +9416,7 @@
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -9451,7 +9467,7 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -9502,7 +9518,7 @@
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -9553,7 +9569,7 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -9604,7 +9620,7 @@
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -9655,7 +9671,7 @@
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -9720,7 +9736,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -9790,7 +9806,7 @@
         <v>6.2769900618376997E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -9860,7 +9876,7 @@
         <v>7.3031816632064184E-9</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -9934,7 +9950,7 @@
         <v>26.594213704935076</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -10004,7 +10020,7 @@
         <v>6.5607985135184749E-9</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -10074,7 +10090,7 @@
         <v>5.8237157645826517E-9</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -10144,7 +10160,7 @@
         <v>4.1795663130837192E-9</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -10214,7 +10230,7 @@
         <v>4.5871559633027526E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -10269,7 +10285,7 @@
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -10324,7 +10340,7 @@
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -10379,7 +10395,7 @@
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -10430,7 +10446,7 @@
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -10481,7 +10497,7 @@
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -10532,7 +10548,7 @@
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -10583,7 +10599,7 @@
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -10634,7 +10650,7 @@
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -10685,7 +10701,7 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -10736,7 +10752,7 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -10787,7 +10803,7 @@
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -10838,7 +10854,7 @@
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -10909,30 +10925,30 @@
       <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -10997,7 +11013,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -11081,7 +11097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -11149,7 +11165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -11233,7 +11249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -11317,7 +11333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -11401,7 +11417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -11485,7 +11501,7 @@
         <v>5.6197500857511838E-10</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -11534,7 +11550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -11585,7 +11601,7 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -11637,7 +11653,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -11686,7 +11702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -11735,7 +11751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -11784,7 +11800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -11833,7 +11849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -11882,7 +11898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -11931,7 +11947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -11980,7 +11996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -12029,7 +12045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -12078,7 +12094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -12127,7 +12143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -12176,7 +12192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -12240,7 +12256,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -12309,7 +12325,7 @@
         <v>4.4212138655335807E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -12378,7 +12394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -12447,7 +12463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -12516,7 +12532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -12585,7 +12601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -12654,7 +12670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <v>28</v>
       </c>
@@ -12723,7 +12739,7 @@
         <v>1.9862967976707304E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -12772,7 +12788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -12821,7 +12837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -12871,7 +12887,7 @@
       </c>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -12920,7 +12936,7 @@
         <v>1.6061787329744499E-7</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -12969,7 +12985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -13018,7 +13034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -13067,7 +13083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -13116,7 +13132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -13165,7 +13181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -13214,7 +13230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -13263,7 +13279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -13312,7 +13328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -13377,25 +13393,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -13433,7 +13449,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -13494,7 +13510,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -13562,7 +13578,7 @@
         <v>7.1205191263816314E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -13630,7 +13646,7 @@
         <v>7.4834154855569742E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -13698,7 +13714,7 @@
         <v>2.0573844793684449E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -13766,7 +13782,7 @@
         <v>3.0503519339716654E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -13824,7 +13840,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -13873,7 +13889,7 @@
         <v>5.9857447747829428E-9</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -13922,7 +13938,7 @@
         <v>2.5901762193934272E-9</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -13971,7 +13987,7 @@
         <v>4.6681470996122009E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -14020,7 +14036,7 @@
         <v>6.2648681882412326E-9</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -14069,7 +14085,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -14118,7 +14134,7 @@
         <v>4.5391131461693942E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -14167,7 +14183,7 @@
         <v>1.7803769385032856E-7</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -14216,7 +14232,7 @@
         <v>5.4110859468596274E-8</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -14265,7 +14281,7 @@
         <v>2.1049365817823592E-9</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -14314,7 +14330,7 @@
         <v>1.4488502372054678E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -14363,7 +14379,7 @@
         <v>1.5160239930406474E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -14412,7 +14428,7 @@
         <v>1.7768347980735624E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -14461,7 +14477,7 @@
         <v>6.249507209650355E-8</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -14510,7 +14526,7 @@
         <v>2.1730325425903627E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -14559,7 +14575,7 @@
         <v>1.6738026719384817E-7</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -14608,7 +14624,7 @@
         <v>2.4192229502593938E-7</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -14657,7 +14673,7 @@
         <v>1.0829418898901413E-7</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -14706,7 +14722,7 @@
         <v>1.6284462085529774E-7</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -14755,7 +14771,7 @@
         <v>1.984838479972653E-7</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -14804,7 +14820,7 @@
         <v>2.0273050531062635E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -14853,7 +14869,7 @@
         <v>1.1501684632164908E-7</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -14902,7 +14918,7 @@
         <v>4.4995057454511165E-8</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -14951,7 +14967,7 @@
         <v>2.4023841356392838E-7</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -15000,7 +15016,7 @@
         <v>1.4169938870962971E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -15049,7 +15065,7 @@
         <v>2.7163596069493577E-7</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -15098,7 +15114,7 @@
         <v>3.0560203715755513E-7</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -15147,7 +15163,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -15196,7 +15212,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -15245,7 +15261,7 @@
         <v>6.8184834679892083E-8</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -15294,7 +15310,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -15343,7 +15359,7 @@
         <v>1.4456958633214434E-7</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -15392,7 +15408,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -15441,7 +15457,7 @@
         <v>1.5607330098029108E-7</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -15490,7 +15506,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -15539,43 +15555,43 @@
         <v>1.958220015922994E-7</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47"/>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55"/>
     </row>
   </sheetData>
@@ -15598,19 +15614,19 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -15628,7 +15644,7 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -15645,7 +15661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -15662,7 +15678,7 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -15679,7 +15695,7 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -15696,7 +15712,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -15713,7 +15729,7 @@
         <v>4.2300000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -15730,7 +15746,7 @@
         <v>7.54</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -15747,7 +15763,7 @@
         <v>13.19</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -15764,7 +15780,7 @@
         <v>14.69</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -15781,7 +15797,7 @@
         <v>17.989999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -15798,7 +15814,7 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="11" customFormat="1">
+    <row r="12" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -15815,7 +15831,7 @@
         <v>22.74</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -15832,7 +15848,7 @@
         <v>24.03</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -15849,7 +15865,7 @@
         <v>24.05</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -15866,7 +15882,7 @@
         <v>24.35</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -15883,7 +15899,7 @@
         <v>24.73</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -15900,7 +15916,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -15917,7 +15933,7 @@
         <v>25.04</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -15934,7 +15950,7 @@
         <v>25.15</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -15951,7 +15967,7 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -15968,7 +15984,7 @@
         <v>25.29</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -15985,7 +16001,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -16002,7 +16018,7 @@
         <v>25.47</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -16019,7 +16035,7 @@
         <v>25.55</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -16036,7 +16052,7 @@
         <v>25.64</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -16053,7 +16069,7 @@
         <v>25.73</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -16070,7 +16086,7 @@
         <v>25.81</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -16087,7 +16103,7 @@
         <v>25.95</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -16104,7 +16120,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -16121,7 +16137,7 @@
         <v>26.22</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -16138,7 +16154,7 @@
         <v>26.55</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -16155,7 +16171,7 @@
         <v>26.67</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -16172,7 +16188,7 @@
         <v>26.83</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -16189,7 +16205,7 @@
         <v>33.43</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -16206,7 +16222,7 @@
         <v>43.43</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -16223,7 +16239,7 @@
         <v>43.51</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -16240,7 +16256,7 @@
         <v>53.52</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -16257,7 +16273,7 @@
         <v>53.61</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -16274,7 +16290,7 @@
         <v>63.61</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -16291,7 +16307,7 @@
         <v>63.78</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -16308,7 +16324,7 @@
         <v>83.82</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -16325,43 +16341,43 @@
         <v>83.96</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55"/>
     </row>
   </sheetData>
@@ -16383,21 +16399,21 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>23</v>
       </c>
@@ -16429,7 +16445,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>24</v>
       </c>
@@ -16461,7 +16477,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>25</v>
       </c>
@@ -16493,7 +16509,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>26</v>
       </c>
@@ -16525,7 +16541,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>27</v>
       </c>
@@ -16557,7 +16573,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>28</v>
       </c>
@@ -16589,7 +16605,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>29</v>
       </c>
@@ -16621,7 +16637,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -16653,7 +16669,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>31</v>
       </c>
@@ -16685,7 +16701,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>32</v>
       </c>
@@ -16717,7 +16733,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>33</v>
       </c>
@@ -16749,7 +16765,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>34</v>
       </c>
@@ -16781,7 +16797,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>35</v>
       </c>
@@ -16813,7 +16829,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>36</v>
       </c>
@@ -16845,7 +16861,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>37</v>
       </c>
@@ -16877,7 +16893,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>38</v>
       </c>
@@ -16909,7 +16925,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>39</v>
       </c>
@@ -16941,7 +16957,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>40</v>
       </c>
@@ -16973,7 +16989,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>41</v>
       </c>
@@ -17008,7 +17024,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>59</v>
       </c>
@@ -17040,7 +17056,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>60</v>
       </c>
@@ -17072,7 +17088,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>61</v>
       </c>
@@ -17104,7 +17120,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>62</v>
       </c>
@@ -17136,7 +17152,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>63</v>
       </c>
@@ -17168,7 +17184,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>64</v>
       </c>
@@ -17200,7 +17216,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>65</v>
       </c>
@@ -17232,7 +17248,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>66</v>
       </c>
@@ -17264,7 +17280,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>67</v>
       </c>
@@ -17296,7 +17312,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>68</v>
       </c>
@@ -17328,7 +17344,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>69</v>
       </c>
@@ -17360,7 +17376,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>70</v>
       </c>
@@ -17392,7 +17408,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>71</v>
       </c>
@@ -17424,7 +17440,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>72</v>
       </c>
@@ -17456,7 +17472,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>73</v>
       </c>
@@ -17488,7 +17504,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>74</v>
       </c>
@@ -17520,7 +17536,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>75</v>
       </c>
@@ -17552,7 +17568,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>76</v>
       </c>
@@ -17584,7 +17600,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>77</v>
       </c>
@@ -17616,7 +17632,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>78</v>
       </c>
@@ -17648,7 +17664,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>79</v>
       </c>
@@ -17680,7 +17696,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>80</v>
       </c>
@@ -17712,7 +17728,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>81</v>
       </c>
@@ -17744,7 +17760,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>82</v>
       </c>
@@ -17776,7 +17792,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Quick save at ven. 23/09/2016_15:54:35,32
</commit_message>
<xml_diff>
--- a/tools/irradiation.xlsx
+++ b/tools/irradiation.xlsx
@@ -296,7 +296,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +345,13 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -484,7 +491,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -537,6 +544,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="100">
@@ -681,6 +691,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1125,11 +1136,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="114493120"/>
-        <c:axId val="114493696"/>
+        <c:axId val="113721344"/>
+        <c:axId val="113721920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="114493120"/>
+        <c:axId val="113721344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1139,12 +1150,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114493696"/>
+        <c:crossAx val="113721920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114493696"/>
+        <c:axId val="113721920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,13 +1166,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114493120"/>
+        <c:crossAx val="113721344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1206,6 +1218,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1530,11 +1543,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="114496000"/>
-        <c:axId val="114496576"/>
+        <c:axId val="113724224"/>
+        <c:axId val="113724800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="114496000"/>
+        <c:axId val="113724224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1544,12 +1557,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114496576"/>
+        <c:crossAx val="113724800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114496576"/>
+        <c:axId val="113724800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,13 +1573,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114496000"/>
+        <c:crossAx val="113724224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1616,6 +1630,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2060,11 +2075,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="114498880"/>
-        <c:axId val="114515968"/>
+        <c:axId val="113727104"/>
+        <c:axId val="113727680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="114498880"/>
+        <c:axId val="113727104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2074,12 +2089,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114515968"/>
+        <c:crossAx val="113727680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114515968"/>
+        <c:axId val="113727680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2090,13 +2105,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114498880"/>
+        <c:crossAx val="113727104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2167,6 +2183,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2491,11 +2508,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="114518272"/>
-        <c:axId val="114518848"/>
+        <c:axId val="114213440"/>
+        <c:axId val="114214016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="114518272"/>
+        <c:axId val="114213440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2505,12 +2522,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114518848"/>
+        <c:crossAx val="114214016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114518848"/>
+        <c:axId val="114214016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2521,13 +2538,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114518272"/>
+        <c:crossAx val="114213440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2706,11 +2724,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="114521152"/>
-        <c:axId val="114521728"/>
+        <c:axId val="114216320"/>
+        <c:axId val="114216896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="114521152"/>
+        <c:axId val="114216320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2719,12 +2737,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114521728"/>
+        <c:crossAx val="114216896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114521728"/>
+        <c:axId val="114216896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2735,7 +2753,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114521152"/>
+        <c:crossAx val="114216320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2762,15 +2780,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4810,7 +4828,7 @@
   <dimension ref="A1:AB55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5604,7 +5622,7 @@
         <v>2694339186.25</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -5663,7 +5681,7 @@
         <v>93.38886304694509</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -5708,7 +5726,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -5761,7 +5779,7 @@
         <v>24.851897123148653</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -5814,7 +5832,7 @@
         <v>1.7593028768513479</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -5859,7 +5877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -5904,7 +5922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -5949,7 +5967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -5994,7 +6012,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -6039,7 +6057,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -6084,7 +6102,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -6129,7 +6147,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -6173,8 +6191,12 @@
       <c r="N28" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -6218,8 +6240,11 @@
       <c r="N29" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -6264,7 +6289,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -6309,7 +6334,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -6356,8 +6381,9 @@
       <c r="O32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T32" s="5"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -6401,8 +6427,9 @@
       <c r="N33" s="1">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T33" s="5"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -6447,7 +6474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -6458,7 +6485,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -6503,7 +6530,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -6514,7 +6541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -6559,7 +6586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -6570,7 +6597,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -6615,7 +6642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -6626,7 +6653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -6671,19 +6698,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="C47"/>
       <c r="D47"/>
@@ -6697,7 +6724,7 @@
       <c r="L47"/>
       <c r="M47"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="C48"/>
       <c r="D48"/>
@@ -8365,10 +8392,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5:AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8396,7 +8423,7 @@
     <col min="22" max="22" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -8461,7 +8488,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -8517,15 +8544,15 @@
         <v>6.3694267515923563E-11</v>
       </c>
       <c r="P2" s="5">
-        <f t="shared" ref="P2:R2" si="0">AVERAGE(F34)</f>
+        <f>AVERAGE(F34)</f>
         <v>0</v>
       </c>
       <c r="Q2" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(G34)</f>
         <v>6.3694267515923563E-11</v>
       </c>
       <c r="R2" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(H34)</f>
         <v>0</v>
       </c>
       <c r="S2" s="5">
@@ -8533,19 +8560,20 @@
         <v>1.2738853503184713E-10</v>
       </c>
       <c r="T2" s="5">
-        <f t="shared" ref="T2:U2" si="1">J34</f>
+        <f t="shared" ref="T2:U2" si="0">J34</f>
         <v>0</v>
       </c>
       <c r="U2" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9.0077296966439174E-11</v>
       </c>
       <c r="V2" s="5">
-        <f t="shared" ref="V2" si="2">L34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+        <f t="shared" ref="V2" si="1">L34</f>
+        <v>0</v>
+      </c>
+      <c r="X2" s="27"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -8602,19 +8630,19 @@
         <v>9.4747406749023928E-9</v>
       </c>
       <c r="P3" s="5">
-        <f t="shared" ref="P3:R3" si="3">AVERAGE(F3,F5,F6,F7,F8,F9,F10,F11,F13)</f>
+        <f>AVERAGE(F3,F5,F6,F7,F8,F9,F10,F11,F13)</f>
         <v>2.3490721165139769E-11</v>
       </c>
       <c r="Q3" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(G3,G5,G6,G7,G8,G9,G10,G11,G13)</f>
         <v>1.6257583550696438E-9</v>
       </c>
       <c r="R3" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(H3,H5,H6,H7,H8,H9,H10,H11,H13)</f>
         <v>2.3490721165139769E-11</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -8671,15 +8699,15 @@
         <v>1.7177345855534705E-7</v>
       </c>
       <c r="P4" s="5">
-        <f t="shared" ref="P4:R4" si="4">AVERAGE(F14,F15,F16,F31)</f>
+        <f>AVERAGE(F14,F15,F16,F31)</f>
         <v>7.1899682620874422E-9</v>
       </c>
       <c r="Q4" s="5">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(G14,G15,G16,G31)</f>
         <v>2.2440983795165841E-8</v>
       </c>
       <c r="R4" s="5">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(H14,H15,H16,H31)</f>
         <v>5.5558446618079027E-9</v>
       </c>
       <c r="S4" s="5">
@@ -8687,19 +8715,19 @@
         <v>1.5432098765432101E-10</v>
       </c>
       <c r="T4" s="5">
-        <f t="shared" ref="T4:U4" si="5">AVERAGE(J14,J15,J16,J31)</f>
+        <f t="shared" ref="T4:U4" si="2">AVERAGE(J14,J15,J16,J31)</f>
         <v>0</v>
       </c>
       <c r="U4" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1.5432098765432101E-10</v>
       </c>
       <c r="V4" s="5">
-        <f t="shared" ref="V4" si="6">AVERAGE(L14,L15,L16,L31)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+        <f t="shared" ref="V4" si="3">AVERAGE(L14,L15,L16,L31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -8756,15 +8784,15 @@
         <v>2.1325966850828727E-7</v>
       </c>
       <c r="P5" s="5">
-        <f t="shared" ref="P5:R5" si="7">AVERAGE(F17)</f>
+        <f>AVERAGE(F17)</f>
         <v>1.878453038674033E-8</v>
       </c>
       <c r="Q5" s="5">
-        <f t="shared" si="7"/>
+        <f>AVERAGE(G17)</f>
         <v>1.5350766839171053E-8</v>
       </c>
       <c r="R5" s="5">
-        <f t="shared" si="7"/>
+        <f>AVERAGE(H17)</f>
         <v>4.5559178183620553E-9</v>
       </c>
       <c r="S5" s="5">
@@ -8772,19 +8800,19 @@
         <v>2.7624309392265192E-8</v>
       </c>
       <c r="T5" s="5">
-        <f t="shared" ref="T5:U5" si="8">AVERAGE(J17)</f>
+        <f t="shared" ref="T5:U5" si="4">AVERAGE(J17)</f>
         <v>0</v>
       </c>
       <c r="U5" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>5.5248618784530382E-9</v>
       </c>
       <c r="V5" s="5">
-        <f t="shared" ref="V5" si="9">AVERAGE(L17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+        <f t="shared" ref="V5" si="5">AVERAGE(L17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -8841,15 +8869,15 @@
         <v>2.5690258150125591E-7</v>
       </c>
       <c r="P6" s="5">
-        <f t="shared" ref="P6:R6" si="10">AVERAGE(F18,F22,F23,F29,F30,F36,F38,F40,F42)</f>
+        <f>AVERAGE(F18,F22,F23,F29,F30,F36,F38,F40,F42)</f>
         <v>2.1310120831168684E-8</v>
       </c>
       <c r="Q6" s="5">
-        <f t="shared" si="10"/>
+        <f>AVERAGE(G18,G22,G23,G29,G30,G36,G38,G40,G42)</f>
         <v>1.9229597646525798E-8</v>
       </c>
       <c r="R6" s="5">
-        <f t="shared" si="10"/>
+        <f>AVERAGE(H18,H22,H23,H29,H30,H36,H38,H40,H42)</f>
         <v>5.4878104158114532E-9</v>
       </c>
       <c r="S6" s="5">
@@ -8857,19 +8885,19 @@
         <v>1.5391353830997568E-7</v>
       </c>
       <c r="T6" s="5">
-        <f t="shared" ref="T6:U6" si="11">AVERAGE(J18,J22,J23,J29,J30,J36,J38,J40)</f>
+        <f t="shared" ref="T6:U6" si="6">AVERAGE(J18,J22,J23,J29,J30,J36,J38,J40)</f>
         <v>4.8723230106987318E-9</v>
       </c>
       <c r="U6" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>1.5098596655809918E-8</v>
       </c>
       <c r="V6" s="5">
-        <f t="shared" ref="V6" si="12">AVERAGE(L18,L22,L23,L29,L30,L36,L38,L40)</f>
+        <f t="shared" ref="V6" si="7">AVERAGE(L18,L22,L23,L29,L30,L36,L38,L40)</f>
         <v>2.6386406738987981E-9</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -8926,15 +8954,15 @@
         <v>3.0780339936267451E-7</v>
       </c>
       <c r="P7" s="5">
-        <f t="shared" ref="P7:R7" si="13">AVERAGE(F19,F20,F21,F24,F25,F26,F27,F28,F32,F33)</f>
+        <f>AVERAGE(F19,F20,F21,F24,F25,F26,F27,F28,F32,F33)</f>
         <v>3.1866601323241053E-8</v>
       </c>
       <c r="Q7" s="5">
-        <f t="shared" si="13"/>
+        <f>AVERAGE(G19,G20,G21,G24,G25,G26,G27,G28,G32,G33)</f>
         <v>2.0765537461360367E-8</v>
       </c>
       <c r="R7" s="5">
-        <f t="shared" si="13"/>
+        <f>AVERAGE(H19,H20,H21,H24,H25,H26,H27,H28,H32,H33)</f>
         <v>6.6351466991058516E-9</v>
       </c>
       <c r="S7" s="5">
@@ -8942,19 +8970,19 @@
         <v>2.5724056772330217E-7</v>
       </c>
       <c r="T7" s="5">
-        <f t="shared" ref="T7:U7" si="14">AVERAGE(J19:J21,J24:J28,J32:J33)</f>
+        <f t="shared" ref="T7:U7" si="8">AVERAGE(J19:J21,J24:J28,J32:J33)</f>
         <v>2.3814660325203556E-8</v>
       </c>
       <c r="U7" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>1.8942638488173582E-8</v>
       </c>
       <c r="V7" s="5">
-        <f t="shared" ref="V7" si="15">AVERAGE(L19:L21,L24:L28,L32:L33)</f>
+        <f t="shared" ref="V7" si="9">AVERAGE(L19:L21,L24:L28,L32:L33)</f>
         <v>5.6749155431643936E-9</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -9007,7 +9035,7 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -9061,7 +9089,7 @@
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -9112,7 +9140,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -9163,7 +9191,7 @@
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -9212,7 +9240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -9263,7 +9291,7 @@
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -9314,7 +9342,7 @@
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -9365,7 +9393,7 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -9790,19 +9818,19 @@
         <v>25.04</v>
       </c>
       <c r="O23" s="5">
-        <f t="shared" ref="O23:R23" si="16">E18</f>
+        <f>E18</f>
         <v>2.4080664294187427E-7</v>
       </c>
       <c r="P23" s="5">
-        <f t="shared" si="16"/>
+        <f>F18</f>
         <v>3.3214709371293001E-8</v>
       </c>
       <c r="Q23" s="5">
-        <f t="shared" si="16"/>
+        <f>G18</f>
         <v>1.6901312987870707E-8</v>
       </c>
       <c r="R23" s="5">
-        <f t="shared" si="16"/>
+        <f>H18</f>
         <v>6.2769900618376997E-9</v>
       </c>
     </row>
@@ -9860,19 +9888,19 @@
         <v>25.36</v>
       </c>
       <c r="O24" s="5">
-        <f t="shared" ref="O24:R24" si="17">E22</f>
+        <f>E22</f>
         <v>2.4480369515011545E-7</v>
       </c>
       <c r="P24" s="5">
-        <f t="shared" si="17"/>
+        <f>F22</f>
         <v>2.3094688221709007E-8</v>
       </c>
       <c r="Q24" s="5">
-        <f t="shared" si="17"/>
+        <f>G22</f>
         <v>2.3777436815212472E-8</v>
       </c>
       <c r="R24" s="5">
-        <f t="shared" si="17"/>
+        <f>H22</f>
         <v>7.3031816632064184E-9</v>
       </c>
     </row>
@@ -9930,19 +9958,19 @@
         <v>26.22</v>
       </c>
       <c r="O25" s="5">
-        <f t="shared" ref="O25:R25" si="18">E30</f>
+        <f>E30</f>
         <v>2.7506426735218507E-7</v>
       </c>
       <c r="P25" s="5">
-        <f t="shared" si="18"/>
+        <f>F30</f>
         <v>1.9280205655526991E-8</v>
       </c>
       <c r="Q25" s="5">
-        <f t="shared" si="18"/>
+        <f>G30</f>
         <v>1.8803006218930324E-8</v>
       </c>
       <c r="R25" s="5">
-        <f t="shared" si="18"/>
+        <f>H30</f>
         <v>4.9781276943540061E-9</v>
       </c>
       <c r="T25" s="5">
@@ -10004,19 +10032,19 @@
         <v>43.51</v>
       </c>
       <c r="O26" s="5">
-        <f t="shared" ref="O26:R26" si="19">E36</f>
+        <f>E36</f>
         <v>2.9166666666666664E-7</v>
       </c>
       <c r="P26" s="5">
-        <f t="shared" si="19"/>
+        <f>F36</f>
         <v>2.2727272727272725E-8</v>
       </c>
       <c r="Q26" s="5">
-        <f t="shared" si="19"/>
+        <f>G36</f>
         <v>2.3503169784073593E-8</v>
       </c>
       <c r="R26" s="5">
-        <f t="shared" si="19"/>
+        <f>H36</f>
         <v>6.5607985135184749E-9</v>
       </c>
     </row>
@@ -10074,19 +10102,19 @@
         <v>53.61</v>
       </c>
       <c r="O27" s="5">
-        <f t="shared" ref="O27:R27" si="20">E38</f>
+        <f>E38</f>
         <v>2.7071823204419894E-7</v>
       </c>
       <c r="P27" s="5">
-        <f t="shared" si="20"/>
+        <f>F38</f>
         <v>1.841620626151013E-8</v>
       </c>
       <c r="Q27" s="5">
-        <f t="shared" si="20"/>
+        <f>G38</f>
         <v>2.2328463449322545E-8</v>
       </c>
       <c r="R27" s="5">
-        <f t="shared" si="20"/>
+        <f>H38</f>
         <v>5.8237157645826517E-9</v>
       </c>
     </row>
@@ -10144,19 +10172,19 @@
         <v>63.78</v>
       </c>
       <c r="O28" s="5">
-        <f t="shared" ref="O28:R28" si="21">E40</f>
+        <f>E40</f>
         <v>2.1588785046728975E-7</v>
       </c>
       <c r="P28" s="5">
-        <f t="shared" si="21"/>
+        <f>F40</f>
         <v>1.8691588785046729E-8</v>
       </c>
       <c r="Q28" s="5">
-        <f t="shared" si="21"/>
+        <f>G40</f>
         <v>1.4204377713617443E-8</v>
       </c>
       <c r="R28" s="5">
-        <f t="shared" si="21"/>
+        <f>H40</f>
         <v>4.1795663130837192E-9</v>
       </c>
     </row>
@@ -10214,19 +10242,19 @@
         <v>83.96</v>
       </c>
       <c r="O29" s="5">
-        <f t="shared" ref="O29:R29" si="22">E42</f>
+        <f>E42</f>
         <v>2.3967889908256879E-7</v>
       </c>
       <c r="P29" s="5">
-        <f t="shared" si="22"/>
+        <f>F42</f>
         <v>1.834862385321101E-8</v>
       </c>
       <c r="Q29" s="5">
-        <f t="shared" si="22"/>
+        <f>G42</f>
         <v>1.657893611789101E-8</v>
       </c>
       <c r="R29" s="5">
-        <f t="shared" si="22"/>
+        <f>H42</f>
         <v>4.5871559633027526E-9</v>
       </c>
     </row>
@@ -10919,10 +10947,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10948,7 +10976,7 @@
     <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -11013,7 +11041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -11097,7 +11125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -11165,7 +11193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -11249,7 +11277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -11333,7 +11361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -11416,8 +11444,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -11500,8 +11532,12 @@
         <f t="shared" si="10"/>
         <v>5.6197500857511838E-10</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -11550,7 +11586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -11601,7 +11637,7 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -11653,7 +11689,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -11702,7 +11738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -11751,7 +11787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -11800,7 +11836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -11849,7 +11885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -11898,7 +11934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -13394,7 +13430,7 @@
   <dimension ref="A1:Q55"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="R11" sqref="R11:U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Quick save at Sat Oct  1 16:47:39 UTC 2016
</commit_message>
<xml_diff>
--- a/tools/irradiation.xlsx
+++ b/tools/irradiation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14385" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27800" windowHeight="14380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -664,7 +664,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -691,7 +691,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -731,22 +730,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>6.3694267515923563E-11</c:v>
+                    <c:v>6.36942675159235E-11</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6257583550696438E-9</c:v>
+                    <c:v>1.62575835506964E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.2440983795165841E-8</c:v>
+                    <c:v>2.24409837951658E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.5350766839171053E-8</c:v>
+                    <c:v>1.53507668391711E-8</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.9229597646525798E-8</c:v>
+                    <c:v>1.92295976465258E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.0765537461360367E-8</c:v>
+                    <c:v>2.07655374613604E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -758,22 +757,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>6.3694267515923563E-11</c:v>
+                    <c:v>6.36942675159235E-11</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6257583550696438E-9</c:v>
+                    <c:v>1.62575835506964E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.2440983795165841E-8</c:v>
+                    <c:v>2.24409837951658E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.5350766839171053E-8</c:v>
+                    <c:v>1.53507668391711E-8</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.9229597646525798E-8</c:v>
+                    <c:v>1.92295976465258E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.0765537461360367E-8</c:v>
+                    <c:v>2.07655374613604E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -784,7 +783,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -802,13 +801,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>40.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -820,22 +819,22 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.3694267515923563E-11</c:v>
+                  <c:v>6.36942675159235E-11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.4747406749023928E-9</c:v>
+                  <c:v>9.4747406749024E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7177345855534705E-7</c:v>
+                  <c:v>1.71773458555347E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1325966850828727E-7</c:v>
+                  <c:v>2.13259668508287E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5690258150125591E-7</c:v>
+                  <c:v>2.56902581501256E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0780339936267451E-7</c:v>
+                  <c:v>3.07803399362674E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -873,22 +872,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.3490721165139769E-11</c:v>
+                    <c:v>2.34907211651398E-11</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.5558446618079027E-9</c:v>
+                    <c:v>5.5558446618079E-9</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.5559178183620553E-9</c:v>
+                    <c:v>4.55591781836205E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.4878104158114532E-9</c:v>
+                    <c:v>5.48781041581145E-9</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>6.6351466991058516E-9</c:v>
+                    <c:v>6.63514669910585E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -900,22 +899,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.3490721165139769E-11</c:v>
+                    <c:v>2.34907211651398E-11</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.5558446618079027E-9</c:v>
+                    <c:v>5.5558446618079E-9</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.5559178183620553E-9</c:v>
+                    <c:v>4.55591781836205E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.4878104158114532E-9</c:v>
+                    <c:v>5.48781041581145E-9</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>6.6351466991058516E-9</c:v>
+                    <c:v>6.63514669910585E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -926,7 +925,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -944,13 +943,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>40.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -962,22 +961,22 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3490721165139769E-11</c:v>
+                  <c:v>2.34907211651398E-11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.1899682620874422E-9</c:v>
+                  <c:v>7.18996826208744E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.878453038674033E-8</c:v>
+                  <c:v>1.87845303867403E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1310120831168684E-8</c:v>
+                  <c:v>2.13101208311687E-8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1866601323241053E-8</c:v>
+                  <c:v>3.1866601323241E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1019,13 +1018,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>40.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1037,19 +1036,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>1.2738853503184713E-10</c:v>
+                  <c:v>1.27388535031847E-10</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>1.5432098765432101E-10</c:v>
+                  <c:v>1.54320987654321E-10</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>2.7624309392265192E-8</c:v>
+                  <c:v>2.76243093922652E-8</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>1.5391353830997568E-7</c:v>
+                  <c:v>1.53913538309976E-7</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>2.5724056772330217E-7</c:v>
+                  <c:v>2.57240567723302E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1091,13 +1090,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>40.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1109,19 +1108,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>4.8723230106987318E-9</c:v>
+                  <c:v>4.87232301069873E-9</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>2.3814660325203556E-8</c:v>
+                  <c:v>2.38146603252035E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1136,11 +1135,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113721344"/>
-        <c:axId val="113721920"/>
+        <c:axId val="2063746136"/>
+        <c:axId val="2063742920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113721344"/>
+        <c:axId val="2063746136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1150,12 +1149,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113721920"/>
+        <c:crossAx val="2063742920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113721920"/>
+        <c:axId val="2063742920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1166,14 +1165,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113721344"/>
+        <c:crossAx val="2063746136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1191,7 +1189,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1218,7 +1216,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1258,25 +1255,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>1.6901312987870707E-8</c:v>
+                    <c:v>1.69013129878707E-8</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.3777436815212472E-8</c:v>
+                    <c:v>2.37774368152125E-8</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.8803006218930324E-8</c:v>
+                    <c:v>1.88030062189303E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.3503169784073593E-8</c:v>
+                    <c:v>2.35031697840736E-8</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.2328463449322545E-8</c:v>
+                    <c:v>2.23284634493225E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.4204377713617443E-8</c:v>
+                    <c:v>1.42043777136174E-8</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.657893611789101E-8</c:v>
+                    <c:v>1.6578936117891E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1288,25 +1285,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>1.6901312987870707E-8</c:v>
+                    <c:v>1.69013129878707E-8</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.3777436815212472E-8</c:v>
+                    <c:v>2.37774368152125E-8</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.8803006218930324E-8</c:v>
+                    <c:v>1.88030062189303E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.3503169784073593E-8</c:v>
+                    <c:v>2.35031697840736E-8</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.2328463449322545E-8</c:v>
+                    <c:v>2.23284634493225E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.4204377713617443E-8</c:v>
+                    <c:v>1.42043777136174E-8</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.657893611789101E-8</c:v>
+                    <c:v>1.6578936117891E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1317,7 +1314,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1356,25 +1353,25 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.4080664294187427E-7</c:v>
+                  <c:v>2.40806642941874E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4480369515011545E-7</c:v>
+                  <c:v>2.44803695150115E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7506426735218507E-7</c:v>
+                  <c:v>2.75064267352185E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9166666666666664E-7</c:v>
+                  <c:v>2.91666666666667E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7071823204419894E-7</c:v>
+                  <c:v>2.70718232044199E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1588785046728975E-7</c:v>
+                  <c:v>2.1588785046729E-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3967889908256879E-7</c:v>
+                  <c:v>2.39678899082569E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1412,25 +1409,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>6.2769900618376997E-9</c:v>
+                    <c:v>6.2769900618377E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.3031816632064184E-9</c:v>
+                    <c:v>7.30318166320642E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.9781276943540061E-9</c:v>
+                    <c:v>4.97812769435401E-9</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.5607985135184749E-9</c:v>
+                    <c:v>6.56079851351847E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.8237157645826517E-9</c:v>
+                    <c:v>5.82371576458265E-9</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>4.1795663130837192E-9</c:v>
+                    <c:v>4.17956631308372E-9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>4.5871559633027526E-9</c:v>
+                    <c:v>4.58715596330275E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1442,25 +1439,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>6.2769900618376997E-9</c:v>
+                    <c:v>6.2769900618377E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.3031816632064184E-9</c:v>
+                    <c:v>7.30318166320642E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.9781276943540061E-9</c:v>
+                    <c:v>4.97812769435401E-9</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.5607985135184749E-9</c:v>
+                    <c:v>6.56079851351847E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.8237157645826517E-9</c:v>
+                    <c:v>5.82371576458265E-9</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>4.1795663130837192E-9</c:v>
+                    <c:v>4.17956631308372E-9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>4.5871559633027526E-9</c:v>
+                    <c:v>4.58715596330275E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1471,7 +1468,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1510,25 +1507,25 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.3214709371293001E-8</c:v>
+                  <c:v>3.3214709371293E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3094688221709007E-8</c:v>
+                  <c:v>2.3094688221709E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9280205655526991E-8</c:v>
+                  <c:v>1.9280205655527E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2727272727272725E-8</c:v>
+                  <c:v>2.27272727272727E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.841620626151013E-8</c:v>
+                  <c:v>1.84162062615101E-8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8691588785046729E-8</c:v>
+                  <c:v>1.86915887850467E-8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.834862385321101E-8</c:v>
+                  <c:v>1.8348623853211E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1543,11 +1540,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113724224"/>
-        <c:axId val="113724800"/>
+        <c:axId val="2134181288"/>
+        <c:axId val="2134178088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113724224"/>
+        <c:axId val="2134181288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1557,12 +1554,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113724800"/>
+        <c:crossAx val="2134178088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113724800"/>
+        <c:axId val="2134178088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1573,14 +1570,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113724224"/>
+        <c:crossAx val="2134181288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1598,7 +1594,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1630,7 +1626,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1670,22 +1665,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.2488554743461749E-9</c:v>
+                    <c:v>1.24885547434617E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.0708351019586504E-8</c:v>
+                    <c:v>2.07083510195865E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.4408881163729623E-9</c:v>
+                    <c:v>9.44088811637296E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2314530656039954E-8</c:v>
+                    <c:v>1.231453065604E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.2244644926995123E-8</c:v>
+                    <c:v>1.22446449269951E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1697,22 +1692,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.2488554743461749E-9</c:v>
+                    <c:v>1.24885547434617E-9</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.0708351019586504E-8</c:v>
+                    <c:v>2.07083510195865E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.4408881163729623E-9</c:v>
+                    <c:v>9.44088811637296E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2314530656039954E-8</c:v>
+                    <c:v>1.231453065604E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.2244644926995123E-8</c:v>
+                    <c:v>1.22446449269951E-8</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1723,7 +1718,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1741,13 +1736,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>40.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1759,22 +1754,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1465588286388024E-8</c:v>
+                  <c:v>1.1465588286388E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.060393649675122E-7</c:v>
+                  <c:v>1.06039364967512E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.066298342541436E-8</c:v>
+                  <c:v>8.06629834254143E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0151070608044769E-7</c:v>
+                  <c:v>1.01510706080448E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.5676789436704994E-8</c:v>
+                  <c:v>9.5676789436705E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1812,22 +1807,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9138682956562178E-9</c:v>
+                    <c:v>1.91386829565622E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.3104946627845505E-10</c:v>
+                    <c:v>3.31049466278455E-10</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.5530200966281132E-9</c:v>
+                    <c:v>2.55302009662811E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1839,22 +1834,22 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9138682956562178E-9</c:v>
+                    <c:v>1.91386829565622E-9</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.3104946627845505E-10</c:v>
+                    <c:v>3.31049466278455E-10</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>2.5530200966281132E-9</c:v>
+                    <c:v>2.55302009662811E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1865,7 +1860,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -1883,13 +1878,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>40.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1901,22 +1896,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.314917127071823E-9</c:v>
+                  <c:v>3.31491712707182E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.7339449541284397E-10</c:v>
+                  <c:v>5.73394495412844E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7084188624970326E-8</c:v>
+                  <c:v>1.70841886249703E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1958,13 +1953,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>40.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1976,19 +1971,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.3694267515923563E-11</c:v>
+                  <c:v>6.36942675159235E-11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9889502762430937E-8</c:v>
+                  <c:v>1.98895027624309E-8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.9642845108846474E-8</c:v>
+                  <c:v>7.96428451088465E-8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.2685460442838195E-8</c:v>
+                  <c:v>9.26854604428382E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2030,13 +2025,13 @@
                   <c:v>30.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
+                  <c:v>40.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>49.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2048,19 +2043,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0403294603750854E-9</c:v>
+                  <c:v>1.04032946037509E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2075,11 +2070,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113727104"/>
-        <c:axId val="113727680"/>
+        <c:axId val="2134096824"/>
+        <c:axId val="2134093672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113727104"/>
+        <c:axId val="2134096824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2089,12 +2084,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113727680"/>
+        <c:crossAx val="2134093672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113727680"/>
+        <c:axId val="2134093672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2105,14 +2100,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113727104"/>
+        <c:crossAx val="2134096824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2130,7 +2124,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2183,7 +2177,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2223,25 +2216,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>9.8200060126057377E-9</c:v>
+                    <c:v>9.82000601260573E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6330410650959527E-8</c:v>
+                    <c:v>1.63304106509595E-8</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.2328615741163802E-8</c:v>
+                    <c:v>1.23286157411638E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.4961396693620555E-8</c:v>
+                    <c:v>1.49613966936206E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>8.0395563243389032E-9</c:v>
+                    <c:v>8.0395563243389E-9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>9.5259447969243979E-9</c:v>
+                    <c:v>9.5259447969244E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2253,25 +2246,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>9.8200060126057377E-9</c:v>
+                    <c:v>9.82000601260573E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6330410650959527E-8</c:v>
+                    <c:v>1.63304106509595E-8</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.2328615741163802E-8</c:v>
+                    <c:v>1.23286157411638E-8</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.4961396693620555E-8</c:v>
+                    <c:v>1.49613966936206E-8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>8.0395563243389032E-9</c:v>
+                    <c:v>8.0395563243389E-9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>9.5259447969243979E-9</c:v>
+                    <c:v>9.5259447969244E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2282,7 +2275,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -2321,25 +2314,25 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>8.4474885844748857E-8</c:v>
+                  <c:v>8.44748858447488E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1547344110854504E-7</c:v>
+                  <c:v>1.15473441108545E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1825192802056555E-7</c:v>
+                  <c:v>1.18251928020566E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2154696132596685E-7</c:v>
+                  <c:v>1.21546961325967E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9158878504672909E-8</c:v>
+                  <c:v>6.91588785046729E-8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.9128440366972472E-8</c:v>
+                  <c:v>7.91284403669725E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2377,25 +2370,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>4.4212138655335807E-9</c:v>
+                    <c:v>4.42121386553358E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.9862967976707304E-9</c:v>
+                    <c:v>1.98629679767073E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2407,25 +2400,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>4.4212138655335807E-9</c:v>
+                    <c:v>4.42121386553358E-9</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.9862967976707304E-9</c:v>
+                    <c:v>1.98629679767073E-9</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2436,7 +2429,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="1"/>
+            <c:val val="1.0"/>
           </c:errBars>
           <c:xVal>
             <c:numRef>
@@ -2475,25 +2468,25 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.7123287671232876E-8</c:v>
+                  <c:v>1.71232876712329E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.440366972477064E-9</c:v>
+                  <c:v>3.44036697247706E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2508,11 +2501,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="114213440"/>
-        <c:axId val="114214016"/>
+        <c:axId val="2134056056"/>
+        <c:axId val="2134052856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="114213440"/>
+        <c:axId val="2134056056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2522,12 +2515,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114214016"/>
+        <c:crossAx val="2134052856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114214016"/>
+        <c:axId val="2134052856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2538,14 +2531,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114213440"/>
+        <c:crossAx val="2134056056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2563,7 +2555,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2629,19 +2621,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>81.388340359171622</c:v>
+                  <c:v>81.38834035917162</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.102856559998202</c:v>
+                  <c:v>51.1028565599982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.775772621870921</c:v>
+                  <c:v>43.77577262187092</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.995380204515513</c:v>
+                  <c:v>27.99538020451551</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2697,19 +2689,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18.611659640828378</c:v>
+                  <c:v>18.61165964082838</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.897143440001798</c:v>
+                  <c:v>48.8971434400018</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56.224227378129093</c:v>
+                  <c:v>56.2242273781291</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.004619795484487</c:v>
+                  <c:v>72.00461979548448</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2724,11 +2716,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="114216320"/>
-        <c:axId val="114216896"/>
+        <c:axId val="2133809240"/>
+        <c:axId val="2133812232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="114216320"/>
+        <c:axId val="2133809240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2737,12 +2729,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114216896"/>
+        <c:crossAx val="2133812232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114216896"/>
+        <c:axId val="2133812232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2753,14 +2745,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114216320"/>
+        <c:crossAx val="2133809240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3233,22 +3224,22 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" style="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1">
       <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
@@ -3282,7 +3273,7 @@
       <c r="L1"/>
       <c r="M1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -3316,7 +3307,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -3352,7 +3343,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -3388,7 +3379,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -3424,7 +3415,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -3460,7 +3451,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -3496,7 +3487,7 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="19">
         <v>7</v>
       </c>
@@ -3532,7 +3523,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="19">
         <v>8</v>
       </c>
@@ -3568,7 +3559,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -3604,7 +3595,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="19">
         <v>10</v>
       </c>
@@ -3640,7 +3631,7 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="19">
         <v>11</v>
       </c>
@@ -3676,7 +3667,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="19">
         <v>12</v>
       </c>
@@ -3712,7 +3703,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="19">
         <v>13</v>
       </c>
@@ -3748,7 +3739,7 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="19">
         <v>14</v>
       </c>
@@ -3784,7 +3775,7 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="19">
         <v>15</v>
       </c>
@@ -3820,7 +3811,7 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="19">
         <v>16</v>
       </c>
@@ -3856,7 +3847,7 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="19">
         <v>17</v>
       </c>
@@ -3892,7 +3883,7 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -3928,7 +3919,7 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="19">
         <v>19</v>
       </c>
@@ -3964,7 +3955,7 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="19">
         <v>20</v>
       </c>
@@ -4000,7 +3991,7 @@
       </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="19">
         <v>21</v>
       </c>
@@ -4036,7 +4027,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -4072,7 +4063,7 @@
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="19">
         <v>23</v>
       </c>
@@ -4108,7 +4099,7 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="19">
         <v>24</v>
       </c>
@@ -4144,7 +4135,7 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="19">
         <v>25</v>
       </c>
@@ -4180,7 +4171,7 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="19">
         <v>26</v>
       </c>
@@ -4216,7 +4207,7 @@
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="19">
         <v>27</v>
       </c>
@@ -4252,7 +4243,7 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="19">
         <v>28</v>
       </c>
@@ -4288,7 +4279,7 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="19">
         <v>29</v>
       </c>
@@ -4324,7 +4315,7 @@
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="19">
         <v>30</v>
       </c>
@@ -4360,7 +4351,7 @@
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="19">
         <v>31</v>
       </c>
@@ -4396,7 +4387,7 @@
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="19">
         <v>32</v>
       </c>
@@ -4432,7 +4423,7 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="19">
         <v>33</v>
       </c>
@@ -4468,7 +4459,7 @@
       </c>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="19">
         <v>34</v>
       </c>
@@ -4504,7 +4495,7 @@
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="19">
         <v>35</v>
       </c>
@@ -4540,7 +4531,7 @@
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="19">
         <v>36</v>
       </c>
@@ -4576,7 +4567,7 @@
       </c>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="19">
         <v>37</v>
       </c>
@@ -4612,7 +4603,7 @@
       </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="19">
         <v>38</v>
       </c>
@@ -4648,7 +4639,7 @@
       </c>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" s="19">
         <v>39</v>
       </c>
@@ -4684,7 +4675,7 @@
       </c>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="19">
         <v>40</v>
       </c>
@@ -4720,7 +4711,7 @@
       </c>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="19">
         <v>41</v>
       </c>
@@ -4756,21 +4747,21 @@
       </c>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="C43"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="C44"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="B45" s="4"/>
       <c r="C45"/>
       <c r="E45" s="5"/>
@@ -4778,38 +4769,38 @@
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="C46"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="C47"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="C48"/>
     </row>
-    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" ht="14.25" customHeight="1">
       <c r="C49"/>
     </row>
-    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" ht="14.25" customHeight="1">
       <c r="C50"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3">
       <c r="C51"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3">
       <c r="C52"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3">
       <c r="C53"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3">
       <c r="C54"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3">
       <c r="C55"/>
     </row>
   </sheetData>
@@ -4831,29 +4822,29 @@
       <selection activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -4909,7 +4900,7 @@
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -4954,7 +4945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -5003,7 +4994,7 @@
       </c>
       <c r="P3" s="8"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -5052,7 +5043,7 @@
       </c>
       <c r="P4" s="9"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -5101,7 +5092,7 @@
       </c>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -5148,7 +5139,7 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -5193,7 +5184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -5238,7 +5229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -5283,7 +5274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -5328,7 +5319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -5373,7 +5364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" s="11" customFormat="1">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -5418,7 +5409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -5463,7 +5454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -5508,7 +5499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -5562,7 +5553,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -5622,7 +5613,7 @@
         <v>2694339186.25</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -5681,7 +5672,7 @@
         <v>93.38886304694509</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -5726,7 +5717,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -5779,7 +5770,7 @@
         <v>24.851897123148653</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -5832,7 +5823,7 @@
         <v>1.7593028768513479</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -5877,7 +5868,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -5922,7 +5913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -5967,7 +5958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -6012,7 +6003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -6057,7 +6048,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -6102,7 +6093,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -6147,7 +6138,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -6196,7 +6187,7 @@
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -6244,7 +6235,7 @@
       <c r="U29" s="5"/>
       <c r="V29" s="5"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -6289,7 +6280,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -6334,7 +6325,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -6383,7 +6374,7 @@
       </c>
       <c r="T32" s="5"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -6429,7 +6420,7 @@
       </c>
       <c r="T33" s="5"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -6474,7 +6465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -6485,7 +6476,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -6530,7 +6521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -6541,7 +6532,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -6586,7 +6577,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -6597,7 +6588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -6642,7 +6633,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -6653,7 +6644,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -6698,19 +6689,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20">
       <c r="A47"/>
       <c r="C47"/>
       <c r="D47"/>
@@ -6724,7 +6715,7 @@
       <c r="L47"/>
       <c r="M47"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20">
       <c r="A48"/>
       <c r="C48"/>
       <c r="D48"/>
@@ -6738,7 +6729,7 @@
       <c r="L48"/>
       <c r="M48"/>
     </row>
-    <row r="49" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="14.25" customHeight="1">
       <c r="A49"/>
       <c r="C49"/>
       <c r="D49"/>
@@ -6752,7 +6743,7 @@
       <c r="L49"/>
       <c r="M49"/>
     </row>
-    <row r="50" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="14.25" customHeight="1">
       <c r="A50"/>
       <c r="C50"/>
       <c r="D50"/>
@@ -6766,7 +6757,7 @@
       <c r="L50"/>
       <c r="M50"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51"/>
       <c r="C51"/>
       <c r="D51"/>
@@ -6780,7 +6771,7 @@
       <c r="L51"/>
       <c r="M51"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13">
       <c r="A52"/>
       <c r="C52"/>
       <c r="D52"/>
@@ -6794,7 +6785,7 @@
       <c r="L52"/>
       <c r="M52"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="A53"/>
       <c r="C53"/>
       <c r="D53"/>
@@ -6808,7 +6799,7 @@
       <c r="L53"/>
       <c r="M53"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="A54"/>
       <c r="C54"/>
       <c r="D54"/>
@@ -6822,7 +6813,7 @@
       <c r="L54"/>
       <c r="M54"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13">
       <c r="A55"/>
       <c r="C55"/>
       <c r="D55"/>
@@ -6854,26 +6845,26 @@
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
     <col min="8" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="12.5" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
+    <col min="14" max="14" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="2" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -6918,7 +6909,7 @@
       </c>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -6938,7 +6929,7 @@
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -6958,7 +6949,7 @@
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -6978,7 +6969,7 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -6998,7 +6989,7 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -7018,7 +7009,7 @@
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -7038,7 +7029,7 @@
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -7058,7 +7049,7 @@
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -7078,7 +7069,7 @@
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -7098,7 +7089,7 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -7119,7 +7110,7 @@
       <c r="N11" s="11"/>
       <c r="O11" s="24"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -7140,7 +7131,7 @@
       <c r="N12" s="11"/>
       <c r="O12" s="24"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -7184,7 +7175,7 @@
       </c>
       <c r="O13" s="24"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -7228,7 +7219,7 @@
       </c>
       <c r="O14" s="24"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -7272,7 +7263,7 @@
       </c>
       <c r="O15" s="24"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -7314,7 +7305,7 @@
       </c>
       <c r="O16" s="24"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -7360,7 +7351,7 @@
       </c>
       <c r="O17" s="24"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -7406,7 +7397,7 @@
       </c>
       <c r="O18" s="24"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -7452,7 +7443,7 @@
       </c>
       <c r="O19" s="24"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -7498,7 +7489,7 @@
       </c>
       <c r="O20" s="24"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -7544,7 +7535,7 @@
       </c>
       <c r="O21" s="24"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -7590,7 +7581,7 @@
       </c>
       <c r="O22" s="24"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -7636,7 +7627,7 @@
       </c>
       <c r="O23" s="24"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -7682,7 +7673,7 @@
       </c>
       <c r="O24" s="24"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -7728,7 +7719,7 @@
       </c>
       <c r="O25" s="24"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -7774,7 +7765,7 @@
       </c>
       <c r="O26" s="24"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -7820,7 +7811,7 @@
       </c>
       <c r="O27" s="24"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -7866,7 +7857,7 @@
       </c>
       <c r="O28" s="24"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -7912,7 +7903,7 @@
       </c>
       <c r="O29" s="24"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -7958,7 +7949,7 @@
       </c>
       <c r="O30" s="24"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -8004,7 +7995,7 @@
       </c>
       <c r="O31" s="24"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -8050,7 +8041,7 @@
       </c>
       <c r="O32" s="24"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -8096,7 +8087,7 @@
       </c>
       <c r="O33" s="24"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -8140,7 +8131,7 @@
       <c r="N34" s="24"/>
       <c r="O34" s="24"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -8164,7 +8155,7 @@
       <c r="N35" s="24"/>
       <c r="O35" s="24"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -8210,7 +8201,7 @@
       </c>
       <c r="O36" s="24"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -8234,7 +8225,7 @@
       <c r="N37" s="24"/>
       <c r="O37" s="24"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -8279,7 +8270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -8302,7 +8293,7 @@
       <c r="M39" s="24"/>
       <c r="N39" s="24"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -8345,7 +8336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -8368,7 +8359,7 @@
       <c r="M41" s="24"/>
       <c r="N41" s="24"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -8398,32 +8389,32 @@
       <selection activeCell="X5" sqref="X5:AA10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -8488,7 +8479,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -8573,7 +8564,7 @@
       </c>
       <c r="X2" s="27"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -8642,7 +8633,7 @@
         <v>2.3490721165139769E-11</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -8727,7 +8718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -8812,7 +8803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -8897,7 +8888,7 @@
         <v>2.6386406738987981E-9</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -8982,7 +8973,7 @@
         <v>5.6749155431643936E-9</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -9035,7 +9026,7 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -9089,7 +9080,7 @@
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -9140,7 +9131,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -9191,7 +9182,7 @@
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -9240,7 +9231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -9291,7 +9282,7 @@
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -9342,7 +9333,7 @@
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -9393,7 +9384,7 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -9444,7 +9435,7 @@
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -9495,7 +9486,7 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -9546,7 +9537,7 @@
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -9597,7 +9588,7 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -9648,7 +9639,7 @@
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -9699,7 +9690,7 @@
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -9764,7 +9755,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -9834,7 +9825,7 @@
         <v>6.2769900618376997E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -9904,7 +9895,7 @@
         <v>7.3031816632064184E-9</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -9978,7 +9969,7 @@
         <v>26.594213704935076</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -10048,7 +10039,7 @@
         <v>6.5607985135184749E-9</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -10118,7 +10109,7 @@
         <v>5.8237157645826517E-9</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -10188,7 +10179,7 @@
         <v>4.1795663130837192E-9</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -10258,7 +10249,7 @@
         <v>4.5871559633027526E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -10313,7 +10304,7 @@
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -10368,7 +10359,7 @@
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -10423,7 +10414,7 @@
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -10474,7 +10465,7 @@
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -10525,7 +10516,7 @@
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -10576,7 +10567,7 @@
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -10627,7 +10618,7 @@
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -10678,7 +10669,7 @@
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -10729,7 +10720,7 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -10780,7 +10771,7 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -10831,7 +10822,7 @@
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -10882,7 +10873,7 @@
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -10953,30 +10944,30 @@
       <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -11041,7 +11032,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -11125,7 +11116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -11193,7 +11184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -11277,7 +11268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -11361,7 +11352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -11449,7 +11440,7 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -11537,7 +11528,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -11586,7 +11577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -11637,7 +11628,7 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -11689,7 +11680,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -11738,7 +11729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -11787,7 +11778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -11836,7 +11827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -11885,7 +11876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -11934,7 +11925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -11983,7 +11974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -12032,7 +12023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -12081,7 +12072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -12130,7 +12121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -12179,7 +12170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -12228,7 +12219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -12292,7 +12283,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -12361,7 +12352,7 @@
         <v>4.4212138655335807E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -12430,7 +12421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -12499,7 +12490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -12568,7 +12559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -12637,7 +12628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -12706,7 +12697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18">
       <c r="A29" s="21">
         <v>28</v>
       </c>
@@ -12775,7 +12766,7 @@
         <v>1.9862967976707304E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -12824,7 +12815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -12873,7 +12864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -12923,7 +12914,7 @@
       </c>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -12972,7 +12963,7 @@
         <v>1.6061787329744499E-7</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -13021,7 +13012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -13070,7 +13061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -13119,7 +13110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -13168,7 +13159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -13217,7 +13208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -13266,7 +13257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -13315,7 +13306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -13364,7 +13355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -13433,21 +13424,21 @@
       <selection activeCell="R11" sqref="R11:U12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -13485,7 +13476,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -13546,7 +13537,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -13614,7 +13605,7 @@
         <v>7.1205191263816314E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -13682,7 +13673,7 @@
         <v>7.4834154855569742E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -13750,7 +13741,7 @@
         <v>2.0573844793684449E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -13818,7 +13809,7 @@
         <v>3.0503519339716654E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -13876,7 +13867,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -13925,7 +13916,7 @@
         <v>5.9857447747829428E-9</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -13974,7 +13965,7 @@
         <v>2.5901762193934272E-9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -14023,7 +14014,7 @@
         <v>4.6681470996122009E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -14072,7 +14063,7 @@
         <v>6.2648681882412326E-9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -14121,7 +14112,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -14170,7 +14161,7 @@
         <v>4.5391131461693942E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -14219,7 +14210,7 @@
         <v>1.7803769385032856E-7</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -14268,7 +14259,7 @@
         <v>5.4110859468596274E-8</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -14317,7 +14308,7 @@
         <v>2.1049365817823592E-9</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -14366,7 +14357,7 @@
         <v>1.4488502372054678E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -14415,7 +14406,7 @@
         <v>1.5160239930406474E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -14464,7 +14455,7 @@
         <v>1.7768347980735624E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -14513,7 +14504,7 @@
         <v>6.249507209650355E-8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -14562,7 +14553,7 @@
         <v>2.1730325425903627E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -14611,7 +14602,7 @@
         <v>1.6738026719384817E-7</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -14660,7 +14651,7 @@
         <v>2.4192229502593938E-7</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -14709,7 +14700,7 @@
         <v>1.0829418898901413E-7</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -14758,7 +14749,7 @@
         <v>1.6284462085529774E-7</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -14807,7 +14798,7 @@
         <v>1.984838479972653E-7</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -14856,7 +14847,7 @@
         <v>2.0273050531062635E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -14905,7 +14896,7 @@
         <v>1.1501684632164908E-7</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -14954,7 +14945,7 @@
         <v>4.4995057454511165E-8</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -15003,7 +14994,7 @@
         <v>2.4023841356392838E-7</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -15052,7 +15043,7 @@
         <v>1.4169938870962971E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -15101,7 +15092,7 @@
         <v>2.7163596069493577E-7</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -15150,7 +15141,7 @@
         <v>3.0560203715755513E-7</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -15199,7 +15190,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -15248,7 +15239,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -15297,7 +15288,7 @@
         <v>6.8184834679892083E-8</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -15346,7 +15337,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -15395,7 +15386,7 @@
         <v>1.4456958633214434E-7</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -15444,7 +15435,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -15493,7 +15484,7 @@
         <v>1.5607330098029108E-7</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -15542,7 +15533,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -15591,43 +15582,43 @@
         <v>1.958220015922994E-7</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="A47"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55"/>
     </row>
   </sheetData>
@@ -15650,19 +15641,19 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -15680,7 +15671,7 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -15697,7 +15688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -15714,7 +15705,7 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -15731,7 +15722,7 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -15748,7 +15739,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -15765,7 +15756,7 @@
         <v>4.2300000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -15782,7 +15773,7 @@
         <v>7.54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -15799,7 +15790,7 @@
         <v>13.19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -15816,7 +15807,7 @@
         <v>14.69</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -15833,7 +15824,7 @@
         <v>17.989999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -15850,7 +15841,7 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="11" customFormat="1">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -15867,7 +15858,7 @@
         <v>22.74</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -15884,7 +15875,7 @@
         <v>24.03</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -15901,7 +15892,7 @@
         <v>24.05</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -15918,7 +15909,7 @@
         <v>24.35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -15935,7 +15926,7 @@
         <v>24.73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -15952,7 +15943,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -15969,7 +15960,7 @@
         <v>25.04</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -15986,7 +15977,7 @@
         <v>25.15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -16003,7 +15994,7 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -16020,7 +16011,7 @@
         <v>25.29</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -16037,7 +16028,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -16054,7 +16045,7 @@
         <v>25.47</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -16071,7 +16062,7 @@
         <v>25.55</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -16088,7 +16079,7 @@
         <v>25.64</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -16105,7 +16096,7 @@
         <v>25.73</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -16122,7 +16113,7 @@
         <v>25.81</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -16139,7 +16130,7 @@
         <v>25.95</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -16156,7 +16147,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -16173,7 +16164,7 @@
         <v>26.22</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -16190,7 +16181,7 @@
         <v>26.55</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -16207,7 +16198,7 @@
         <v>26.67</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -16224,7 +16215,7 @@
         <v>26.83</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -16241,7 +16232,7 @@
         <v>33.43</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -16258,7 +16249,7 @@
         <v>43.43</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -16275,7 +16266,7 @@
         <v>43.51</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -16292,7 +16283,7 @@
         <v>53.52</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -16309,7 +16300,7 @@
         <v>53.61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -16326,7 +16317,7 @@
         <v>63.61</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -16343,7 +16334,7 @@
         <v>63.78</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -16360,7 +16351,7 @@
         <v>83.82</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -16377,43 +16368,43 @@
         <v>83.96</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55"/>
     </row>
   </sheetData>
@@ -16435,21 +16426,21 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1">
         <v>23</v>
       </c>
@@ -16481,7 +16472,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>24</v>
       </c>
@@ -16513,7 +16504,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>25</v>
       </c>
@@ -16545,7 +16536,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>26</v>
       </c>
@@ -16577,7 +16568,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>27</v>
       </c>
@@ -16609,7 +16600,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>28</v>
       </c>
@@ -16641,7 +16632,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>29</v>
       </c>
@@ -16673,7 +16664,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>30</v>
       </c>
@@ -16705,7 +16696,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>31</v>
       </c>
@@ -16737,7 +16728,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>32</v>
       </c>
@@ -16769,7 +16760,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>33</v>
       </c>
@@ -16801,7 +16792,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>34</v>
       </c>
@@ -16833,7 +16824,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>35</v>
       </c>
@@ -16865,7 +16856,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>36</v>
       </c>
@@ -16897,7 +16888,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>37</v>
       </c>
@@ -16929,7 +16920,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>38</v>
       </c>
@@ -16961,7 +16952,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>39</v>
       </c>
@@ -16993,7 +16984,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>40</v>
       </c>
@@ -17025,7 +17016,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>41</v>
       </c>
@@ -17060,7 +17051,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>59</v>
       </c>
@@ -17092,7 +17083,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>60</v>
       </c>
@@ -17124,7 +17115,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>61</v>
       </c>
@@ -17156,7 +17147,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>62</v>
       </c>
@@ -17188,7 +17179,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>63</v>
       </c>
@@ -17220,7 +17211,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>64</v>
       </c>
@@ -17252,7 +17243,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>65</v>
       </c>
@@ -17284,7 +17275,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>66</v>
       </c>
@@ -17316,7 +17307,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>67</v>
       </c>
@@ -17348,7 +17339,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>68</v>
       </c>
@@ -17380,7 +17371,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>69</v>
       </c>
@@ -17412,7 +17403,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>70</v>
       </c>
@@ -17444,7 +17435,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>71</v>
       </c>
@@ -17476,7 +17467,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>72</v>
       </c>
@@ -17508,7 +17499,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>73</v>
       </c>
@@ -17540,7 +17531,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>74</v>
       </c>
@@ -17572,7 +17563,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>75</v>
       </c>
@@ -17604,7 +17595,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>76</v>
       </c>
@@ -17636,7 +17627,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>77</v>
       </c>
@@ -17668,7 +17659,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>78</v>
       </c>
@@ -17700,7 +17691,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>79</v>
       </c>
@@ -17732,7 +17723,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>80</v>
       </c>
@@ -17764,7 +17755,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>81</v>
       </c>
@@ -17796,7 +17787,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>82</v>
       </c>
@@ -17828,7 +17819,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>83</v>
       </c>

</xml_diff>